<commit_message>
Use heavy-duty rather than light-duty trucks as basis of survival curve for industrial equipment
</commit_message>
<xml_diff>
--- a/InputData/indst/IESD/Industrial Equipment Survival Data.xlsx
+++ b/InputData/indst/IESD/Industrial Equipment Survival Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\indst\IESD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514E6E3A-DE1F-4096-9F59-DCD0EC777ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925559C1-3E22-44E0-A5DB-1C1F39487FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4608" yWindow="276" windowWidth="23316" windowHeight="18012" xr2:uid="{F6F8D70B-4981-4594-95C7-E07791D5C609}"/>
+    <workbookView xWindow="7296" yWindow="1044" windowWidth="30240" windowHeight="17220" xr2:uid="{F6F8D70B-4981-4594-95C7-E07791D5C609}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -140,18 +140,12 @@
     <t>To estimate a survival curve for heterogenous mixes of industrial equipment in each ISIC code,</t>
   </si>
   <si>
-    <t>we use a Weibull function to curve fit survival curve data for light commerical trucks from the</t>
-  </si>
-  <si>
     <t>MOVE3 model.  We extend our curve fit to 50 years to avoid a discontinuity in the MOVES3 data</t>
   </si>
   <si>
     <t>where they retire an unusually large share of the remaining stock in year 30.</t>
   </si>
   <si>
-    <t xml:space="preserve">After 50 years, the share of surviving equipment from the curve fit would be just 0.035%.  </t>
-  </si>
-  <si>
     <t>so that we can capture the full lifetime of all industrial equipment and avoid problems with a</t>
   </si>
   <si>
@@ -837,16 +831,23 @@
   </si>
   <si>
     <t>We set this to zero and smoothly adjust the remainder of the Weibull curve accordingly,</t>
+  </si>
+  <si>
+    <t>we use a Weibull function to curve fit survival curve data for heavy-duty commerical trucks from the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After 50 years, the share of surviving equipment from the curve fit would be just 0.5%.  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -883,6 +884,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -1005,10 +1013,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1057,9 +1066,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1154,154 +1165,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>6.0192694283551618E-2</c:v>
+                  <c:v>4.9941081907415655E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0035289835080566E-2</c:v>
+                  <c:v>4.9852160520590598E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9544449970861169E-2</c:v>
+                  <c:v>4.9581767885936025E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8715306239949035E-2</c:v>
+                  <c:v>4.9124221909465797E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.755505173321445E-2</c:v>
+                  <c:v>4.8479967596651581E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.6078928671239994E-2</c:v>
+                  <c:v>4.7653108874577611E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.4308830141498857E-2</c:v>
+                  <c:v>4.6650707228810789E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.2272253912054589E-2</c:v>
+                  <c:v>4.5482377562410338E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0001290290909842E-2</c:v>
+                  <c:v>4.415995931128211E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.7531575760139111E-2</c:v>
+                  <c:v>4.2697200818370286E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.4901211387096983E-2</c:v>
+                  <c:v>4.1109437479695428E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.2149668897197547E-2</c:v>
+                  <c:v>3.9413259417212916E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.9316716243030805E-2</c:v>
+                  <c:v>3.7626170965051685E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.644139662204475E-2</c:v>
+                  <c:v>3.576624732108951E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.356109312408851E-2</c:v>
+                  <c:v>3.3851795121837433E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.0710706913111802E-2</c:v>
+                  <c:v>3.1901024168767632E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.7921970919144796E-2</c:v>
+                  <c:v>2.993173740221319E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.5222914095973024E-2</c:v>
+                  <c:v>2.7961045665188474E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.2637483954423183E-2</c:v>
+                  <c:v>2.6005112940459322E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0185327813132176E-2</c:v>
+                  <c:v>2.4078936668643976E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.7881726451497666E-2</c:v>
+                  <c:v>2.2196166538662569E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.573766795613173E-2</c:v>
+                  <c:v>2.0368963852577183E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.3760044783996846E-2</c:v>
+                  <c:v>1.8607902266875063E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.1951953586143727E-2</c:v>
+                  <c:v>1.6921909457347849E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.0313075211417583E-2</c:v>
+                  <c:v>1.5318248093427685E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.8401115140645629E-3</c:v>
+                  <c:v>1.3802533480304061E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.527256017871682E-3</c:v>
+                  <c:v>1.2378784364243197E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.3666769742583788E-3</c:v>
+                  <c:v>1.1049502719360317E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.3489936803957595E-3</c:v>
+                  <c:v>9.8157778538863864E-3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.4637298593843263E-3</c:v>
+                  <c:v>8.6774098924622765E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.6997312058400008E-3</c:v>
+                  <c:v>7.6330476012252636E-3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0455376364937939E-3</c:v>
+                  <c:v>6.680335609903592E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.4897041513629674E-3</c:v>
+                  <c:v>5.8160663291400979E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.0210673365311312E-3</c:v>
+                  <c:v>5.0363322365897644E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.6289572953558926E-3</c:v>
+                  <c:v>4.336674683824729E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.3033570947362115E-3</c:v>
+                  <c:v>3.712225928283366E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.0350136122116973E-3</c:v>
+                  <c:v>3.1578416911779905E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.155049608578695E-4</c:v>
+                  <c:v>2.6682221557343786E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6.3727047624667003E-4</c:v>
+                  <c:v>2.2380199253197314E-3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.9360962132467118E-4</c:v>
+                  <c:v>1.8619340363392101E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.7865616556427702E-4</c:v>
+                  <c:v>1.53478964868602E-3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.8733369794371315E-4</c:v>
+                  <c:v>1.2516035037630799E-3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.1529801555439907E-4</c:v>
+                  <c:v>1.0076356377359192E-3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.5887126440472155E-4</c:v>
+                  <c:v>7.9842816094936842E-4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.1497196278900563E-4</c:v>
+                  <c:v>6.1983216233548084E-4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>8.1044267182817299E-5</c:v>
+                  <c:v>4.6802397241129008E-4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5.4989091543849397E-5</c:v>
+                  <c:v>3.395121250354253E-4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.5098997072430095E-5</c:v>
+                  <c:v>2.3113640341805268E-4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.9998153758015452E-5</c:v>
+                  <c:v>1.4006034831220358E-4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>8.5881503200550279E-6</c:v>
+                  <c:v>6.3758554998347974E-5</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>0</c:v>
@@ -1764,94 +1775,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.99099999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99099999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99099999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98599999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98099999999999998</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.97599999999999998</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.97</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.96399999999999997</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.95799999999999996</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.95199999999999996</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.94599999999999995</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>0.94</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.93500000000000005</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.92900000000000005</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.91300000000000003</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.90800000000000003</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.90300000000000002</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.89800000000000002</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.89400000000000002</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.89100000000000001</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.88800000000000001</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.88500000000000001</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.88300000000000001</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.88</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.879</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.877</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.875</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.875</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.873</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.872</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0.3</c:v>
@@ -2076,94 +2087,94 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99099999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98208099999999998</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96833186599999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.94993356054599998</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.92713515509289601</c:v>
+                  <c:v>0.97019999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.89932110044010916</c:v>
+                  <c:v>0.95079599999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.86694554082426523</c:v>
+                  <c:v>0.92227211999999992</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.83053382810964604</c:v>
+                  <c:v>0.8946039563999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.79066820436038299</c:v>
+                  <c:v>0.86776583770799987</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.7479721213249223</c:v>
+                  <c:v>0.83305520419967982</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.70309379404542693</c:v>
+                  <c:v>0.79973299603169257</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.65739269743247419</c:v>
+                  <c:v>0.75974634623010795</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.61071781591476859</c:v>
+                  <c:v>0.72175902891860255</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.55758536593018371</c:v>
+                  <c:v>0.68567107747267242</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.50628751226460678</c:v>
+                  <c:v>0.64453081282431202</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.45717762357493991</c:v>
+                  <c:v>0.60585896405485329</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.41054550597029604</c:v>
+                  <c:v>0.56344883657101363</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.36702768233744465</c:v>
+                  <c:v>0.52400741801104267</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.32702166496266316</c:v>
+                  <c:v>0.48208682457015928</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.2903952384868449</c:v>
+                  <c:v>0.44351987860454656</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.25699978606085772</c:v>
+                  <c:v>0.40803828831618283</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.22693081109173738</c:v>
+                  <c:v>0.37131484236772638</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.19969911376072888</c:v>
+                  <c:v>0.33789650655463099</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.17553552099568068</c:v>
+                  <c:v>0.30748582096471422</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.15394465191321197</c:v>
+                  <c:v>0.27673723886824281</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.13470157042406047</c:v>
+                  <c:v>0.24906351498141854</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.11786387412105291</c:v>
+                  <c:v>0.22415716348327669</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.1028951621076792</c:v>
+                  <c:v>0.19949987550011625</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8.9724581357896266E-2</c:v>
+                  <c:v>0.17755488919510345</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.6917374407368879E-2</c:v>
+                  <c:v>5.3266466758531035E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2202,9 +2213,7 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent3"/>
@@ -2385,154 +2394,154 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99739212515354392</c:v>
+                  <c:v>0.99831675588711721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98924478377020841</c:v>
+                  <c:v>0.99299980499619667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.97547709475632682</c:v>
+                  <c:v>0.98393537137827769</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.95620855917354664</c:v>
+                  <c:v>0.97113236564271588</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9316924007853824</c:v>
+                  <c:v>0.95467296316352146</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9022923362809403</c:v>
+                  <c:v>0.93469856026807085</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.86846519465567973</c:v>
+                  <c:v>0.911401681881576</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.83074410220315842</c:v>
+                  <c:v>0.88501939607412372</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.78972109891259246</c:v>
+                  <c:v>0.85582699409730667</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.74602916969698607</c:v>
+                  <c:v>0.82413154571082692</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.7003240706390983</c:v>
+                  <c:v>0.79026524479839177</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.653266479136134</c:v>
+                  <c:v>0.75457859105805325</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.60550503200212358</c:v>
+                  <c:v>0.71743351493239338</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.55766078616588688</c:v>
+                  <c:v>0.67919658109746339</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.51031356554733853</c:v>
+                  <c:v>0.64023241524371066</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.46399055920833854</c:v>
+                  <c:v>0.60089749623889543</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.41915742089838504</c:v>
+                  <c:v>0.56153444467433955</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.37621199808238615</c:v>
+                  <c:v>0.52246692159518826</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.33548069779147327</c:v>
+                  <c:v>0.48399522967902553</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.2972173843787802</c:v>
+                  <c:v>0.44639268476921745</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.26160460635360461</c:v>
+                  <c:v>0.4099027998534206</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.22875687025273661</c:v>
+                  <c:v>0.37473729754723328</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.1987256217057094</c:v>
+                  <c:v>0.34107494201536037</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.1715055585548676</c:v>
+                  <c:v>0.30906115800942446</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.14704188767634285</c:v>
+                  <c:v>0.27880838412656883</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.12523814427017732</c:v>
+                  <c:v>0.25039709011459887</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.10596421705503067</c:v>
+                  <c:v>0.22387737448999978</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8.9064261489625096E-2</c:v>
+                  <c:v>0.19927104911966265</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.4364231919015422E-2</c:v>
+                  <c:v>0.17657411178033777</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6.1678818389612644E-2</c:v>
+                  <c:v>0.15575950591235288</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.0817630964475224E-2</c:v>
+                  <c:v>0.13678006853521585</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.1590530289999483E-2</c:v>
+                  <c:v>0.1195715721785825</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.3812055089708859E-2</c:v>
+                  <c:v>0.10405577419740442</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.7304943043493068E-2</c:v>
+                  <c:v>9.0143396421134003E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.1902779718167675E-2</c:v>
+                  <c:v>7.773696914395567E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.7451840104900196E-2</c:v>
+                  <c:v>6.6733485410649274E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.3812208770020096E-2</c:v>
+                  <c:v>5.7026823836338725E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.085827803774464E-2</c:v>
+                  <c:v>4.8509910316327787E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.4787297965790431E-3</c:v>
+                  <c:v>4.1076600502268801E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.5761065295036891E-3</c:v>
+                  <c:v>3.4623275491463823E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.0660722372383171E-3</c:v>
+                  <c:v>2.9050152531782669E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.8764553222113696E-3</c:v>
+                  <c:v>2.4262320506897139E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.9461544491962144E-3</c:v>
+                  <c:v>2.0170516439616759E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.2239760017190857E-3</c:v>
+                  <c:v>1.6691664214857793E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.6674589543207441E-3</c:v>
+                  <c:v>1.3749200223324487E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.2417305360230557E-3</c:v>
+                  <c:v>1.1273212760904316E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>9.1842453361701271E-4</c:v>
+                  <c:v>9.2004229263573656E-3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6.7468385411284526E-4</c:v>
+                  <c:v>7.47403460837337E-3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.9226024838955329E-4</c:v>
+                  <c:v>6.0434801255350168E-3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.5671696845152034E-4</c:v>
+                  <c:v>4.8640863672232415E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2842,151 +2851,151 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6150091858251345E-3</c:v>
+                  <c:v>1.7805258402272539E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.1758556603583749E-3</c:v>
+                  <c:v>5.4238899945548685E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3924786127303026E-2</c:v>
+                  <c:v>9.2281093631599309E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9760682197466944E-2</c:v>
+                  <c:v>1.3114799334665243E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5647150293891575E-2</c:v>
+                  <c:v>1.7055678109221407E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1564414151316167E-2</c:v>
+                  <c:v>2.1035388234692781E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7499909759390417E-2</c:v>
+                  <c:v>2.5044200523478943E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.3444914867561142E-2</c:v>
+                  <c:v>2.9075398473037677E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.939301598822373E-2</c:v>
+                  <c:v>3.3124090595303565E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.533930510353504E-2</c:v>
+                  <c:v>3.7186590882832007E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.1279916619134567E-2</c:v>
+                  <c:v>4.1260064998950227E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.7211741593422109E-2</c:v>
+                  <c:v>4.5342315722834106E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.3132242357491523E-2</c:v>
+                  <c:v>4.943164813899685E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.9039327933272382E-2</c:v>
+                  <c:v>5.3526784123175901E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.4931268491098139E-2</c:v>
+                  <c:v>5.7626809628520313E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.0806636325794512E-2</c:v>
+                  <c:v>6.1731145562481743E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.6664265964160612E-2</c:v>
+                  <c:v>6.5839537162283163E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.10250322907623978</c:v>
+                  <c:v>6.9952059309580428E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.10832282183956567</c:v>
+                  <c:v>7.4069136951086217E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.11412256382261145</c:v>
+                  <c:v>7.8191581127134355E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.11990220861399896</c:v>
+                  <c:v>8.2320642301122543E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.12566176752791119</c:v>
+                  <c:v>8.6458083899014881E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.13140154892198885</c:v>
+                  <c:v>9.0606280350501611E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.13712221712659151</c:v>
+                  <c:v>9.4768345615028685E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.14282487688272696</c:v>
+                  <c:v>9.8948300346039089E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.14851119175410132</c:v>
+                  <c:v>0.10315128871757681</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.15418354854116612</c:v>
+                  <c:v>0.10738385981765565</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.1598452847501603</c:v>
+                  <c:v>0.11165433384728421</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.1655010033487147</c:v>
+                  <c:v>0.11597328081068911</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.17115700940954851</c:v>
+                  <c:v>0.12035414993409603</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.17682191839060279</c:v>
+                  <c:v>0.1248141032382323</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.18250750818851658</c:v>
+                  <c:v>0.12937512892050151</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.18822992064148872</c:v>
+                  <c:v>0.13406554334562018</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.19401136918487752</c:v>
+                  <c:v>0.13892204086178234</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.1998825884189582</c:v>
+                  <c:v>0.14399252908466512</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.2058863864770879</c:v>
+                  <c:v>0.14934011232493538</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.2120828641903218</c:v>
+                  <c:v>0.15504879070140029</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.21855720463515754</c:v>
+                  <c:v>0.16123178854882186</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.22543152441035361</c:v>
+                  <c:v>0.16804403067447776</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.23288333694124572</c:v>
+                  <c:v>0.17570138429629648</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.24117517665260854</c:v>
+                  <c:v>0.184511372724845</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.25070391292366057</c:v>
+                  <c:v>0.19492424341546283</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.26208672199962879</c:v>
+                  <c:v>0.20762214926878136</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.27631996119753455</c:v>
+                  <c:v>0.22368449329433546</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.29509538485005954</c:v>
+                  <c:v>0.244918220042324</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.32149313633984</c:v>
+                  <c:v>0.27458389943951667</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.36170982122078776</c:v>
+                  <c:v>0.31921016548691594</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.43023574956437149</c:v>
+                  <c:v>0.39403596213756642</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.57055284082847824</c:v>
+                  <c:v>0.54477797773124181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4125,154 +4134,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>8.5881503200550279E-6</c:v>
+                  <c:v>6.3758554998347974E-5</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.9998153758015452E-5</c:v>
+                  <c:v>1.4006034831220358E-4</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>3.5098997072430095E-5</c:v>
+                  <c:v>2.3113640341805268E-4</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>5.4989091543849397E-5</c:v>
+                  <c:v>3.395121250354253E-4</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>8.1044267182817299E-5</c:v>
+                  <c:v>4.6802397241129008E-4</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.1497196278900563E-4</c:v>
+                  <c:v>6.1983216233548084E-4</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.5887126440472155E-4</c:v>
+                  <c:v>7.9842816094936842E-4</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2.1529801555439907E-4</c:v>
+                  <c:v>1.0076356377359192E-3</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2.8733369794371315E-4</c:v>
+                  <c:v>1.2516035037630799E-3</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>3.7865616556427702E-4</c:v>
+                  <c:v>1.53478964868602E-3</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>4.9360962132467118E-4</c:v>
+                  <c:v>1.8619340363392101E-3</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>6.3727047624667003E-4</c:v>
+                  <c:v>2.2380199253197314E-3</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>8.155049608578695E-4</c:v>
+                  <c:v>2.6682221557343786E-3</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1.0350136122116973E-3</c:v>
+                  <c:v>3.1578416911779905E-3</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.3033570947362115E-3</c:v>
+                  <c:v>3.712225928283366E-3</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.6289572953558926E-3</c:v>
+                  <c:v>4.336674683824729E-3</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2.0210673365311312E-3</c:v>
+                  <c:v>5.0363322365897644E-3</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2.4897041513629674E-3</c:v>
+                  <c:v>5.8160663291400979E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>3.0455376364937939E-3</c:v>
+                  <c:v>6.680335609903592E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>3.6997312058400008E-3</c:v>
+                  <c:v>7.6330476012252636E-3</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>4.4637298593843263E-3</c:v>
+                  <c:v>8.6774098924622765E-3</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>5.3489936803957595E-3</c:v>
+                  <c:v>9.8157778538863864E-3</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>6.3666769742583788E-3</c:v>
+                  <c:v>1.1049502719360317E-2</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>7.527256017871682E-3</c:v>
+                  <c:v>1.2378784364243197E-2</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>8.8401115140645629E-3</c:v>
+                  <c:v>1.3802533480304061E-2</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1.0313075211417583E-2</c:v>
+                  <c:v>1.5318248093427685E-2</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1.1951953586143727E-2</c:v>
+                  <c:v>1.6921909457347849E-2</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1.3760044783996846E-2</c:v>
+                  <c:v>1.8607902266875063E-2</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1.573766795613173E-2</c:v>
+                  <c:v>2.0368963852577183E-2</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1.7881726451497666E-2</c:v>
+                  <c:v>2.2196166538662569E-2</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>2.0185327813132176E-2</c:v>
+                  <c:v>2.4078936668643976E-2</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>2.2637483954423183E-2</c:v>
+                  <c:v>2.6005112940459322E-2</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>2.5222914095973024E-2</c:v>
+                  <c:v>2.7961045665188474E-2</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>2.7921970919144796E-2</c:v>
+                  <c:v>2.993173740221319E-2</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>3.0710706913111802E-2</c:v>
+                  <c:v>3.1901024168767632E-2</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>3.356109312408851E-2</c:v>
+                  <c:v>3.3851795121837433E-2</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>3.644139662204475E-2</c:v>
+                  <c:v>3.576624732108951E-2</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>3.9316716243030805E-2</c:v>
+                  <c:v>3.7626170965051685E-2</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>4.2149668897197547E-2</c:v>
+                  <c:v>3.9413259417212916E-2</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>4.4901211387096983E-2</c:v>
+                  <c:v>4.1109437479695428E-2</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>4.7531575760139111E-2</c:v>
+                  <c:v>4.2697200818370286E-2</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>5.0001290290909842E-2</c:v>
+                  <c:v>4.415995931128211E-2</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>5.2272253912054589E-2</c:v>
+                  <c:v>4.5482377562410338E-2</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>5.4308830141498857E-2</c:v>
+                  <c:v>4.6650707228810789E-2</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>5.6078928671239994E-2</c:v>
+                  <c:v>4.7653108874577611E-2</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>5.755505173321445E-2</c:v>
+                  <c:v>4.8479967596651581E-2</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>5.8715306239949035E-2</c:v>
+                  <c:v>4.9124221909465797E-2</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>5.9544449970861169E-2</c:v>
+                  <c:v>4.9581767885936025E-2</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>6.0035289835080566E-2</c:v>
+                  <c:v>4.9852160520590598E-2</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>6.0192694283551618E-2</c:v>
+                  <c:v>4.9941081907415655E-2</c:v>
                 </c:pt>
                 <c:pt idx="130">
                   <c:v>0</c:v>
@@ -7399,12 +7408,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -7447,57 +7456,57 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B24" s="12"/>
     </row>
@@ -7510,17 +7519,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B12B9A-7BC4-4CDD-8298-A2C7A60D90EB}">
   <dimension ref="A1:AZ12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="53.44140625" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -7681,95 +7691,95 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <f t="array" ref="B2:AF2">TRANSPOSE('MOVES3 Table C-1'!D3:D33)</f>
-        <v>0.99099999999999999</v>
+        <f t="array" ref="B2:AF2">TRANSPOSE('MOVES3 Table C-1'!E3:E33)</f>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0.99099999999999999</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0.99099999999999999</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.98599999999999999</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0.98099999999999998</v>
+        <v>0.99</v>
       </c>
       <c r="G2">
-        <v>0.97599999999999998</v>
+        <v>0.98</v>
       </c>
       <c r="H2">
+        <v>0.98</v>
+      </c>
+      <c r="I2">
         <v>0.97</v>
       </c>
-      <c r="I2">
-        <v>0.96399999999999997</v>
-      </c>
       <c r="J2">
-        <v>0.95799999999999996</v>
+        <v>0.97</v>
       </c>
       <c r="K2">
-        <v>0.95199999999999996</v>
+        <v>0.97</v>
       </c>
       <c r="L2">
-        <v>0.94599999999999995</v>
+        <v>0.96</v>
       </c>
       <c r="M2">
+        <v>0.96</v>
+      </c>
+      <c r="N2">
+        <v>0.95</v>
+      </c>
+      <c r="O2">
+        <v>0.95</v>
+      </c>
+      <c r="P2">
+        <v>0.95</v>
+      </c>
+      <c r="Q2">
         <v>0.94</v>
       </c>
-      <c r="N2">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="O2">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="P2">
-        <v>0.91300000000000003</v>
-      </c>
-      <c r="Q2">
-        <v>0.90800000000000003</v>
-      </c>
       <c r="R2">
-        <v>0.90300000000000002</v>
+        <v>0.94</v>
       </c>
       <c r="S2">
-        <v>0.89800000000000002</v>
+        <v>0.93</v>
       </c>
       <c r="T2">
-        <v>0.89400000000000002</v>
+        <v>0.93</v>
       </c>
       <c r="U2">
-        <v>0.89100000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="V2">
-        <v>0.88800000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="W2">
-        <v>0.88500000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="X2">
-        <v>0.88300000000000001</v>
+        <v>0.91</v>
       </c>
       <c r="Y2">
-        <v>0.88</v>
+        <v>0.91</v>
       </c>
       <c r="Z2">
-        <v>0.879</v>
+        <v>0.91</v>
       </c>
       <c r="AA2">
-        <v>0.877</v>
+        <v>0.9</v>
       </c>
       <c r="AB2">
-        <v>0.875</v>
+        <v>0.9</v>
       </c>
       <c r="AC2">
-        <v>0.875</v>
+        <v>0.9</v>
       </c>
       <c r="AD2">
-        <v>0.873</v>
+        <v>0.89</v>
       </c>
       <c r="AE2">
-        <v>0.872</v>
+        <v>0.89</v>
       </c>
       <c r="AF2">
         <v>0.3</v>
@@ -7784,123 +7794,123 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:AF3" si="0">B3*C2</f>
-        <v>0.99099999999999999</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
-        <v>0.98208099999999998</v>
+        <f>C3*D2</f>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>0.96833186599999999</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>0.94993356054599998</v>
+        <v>0.99</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>0.92713515509289601</v>
+        <v>0.97019999999999995</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>0.89932110044010916</v>
+        <v>0.95079599999999997</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
-        <v>0.86694554082426523</v>
+        <v>0.92227211999999992</v>
       </c>
       <c r="J3">
         <f t="shared" si="0"/>
-        <v>0.83053382810964604</v>
+        <v>0.8946039563999999</v>
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
-        <v>0.79066820436038299</v>
+        <v>0.86776583770799987</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>0.7479721213249223</v>
+        <v>0.83305520419967982</v>
       </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>0.70309379404542693</v>
+        <v>0.79973299603169257</v>
       </c>
       <c r="N3">
         <f t="shared" si="0"/>
-        <v>0.65739269743247419</v>
+        <v>0.75974634623010795</v>
       </c>
       <c r="O3">
         <f t="shared" si="0"/>
-        <v>0.61071781591476859</v>
+        <v>0.72175902891860255</v>
       </c>
       <c r="P3">
         <f t="shared" si="0"/>
-        <v>0.55758536593018371</v>
+        <v>0.68567107747267242</v>
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
-        <v>0.50628751226460678</v>
+        <v>0.64453081282431202</v>
       </c>
       <c r="R3">
         <f t="shared" si="0"/>
-        <v>0.45717762357493991</v>
+        <v>0.60585896405485329</v>
       </c>
       <c r="S3">
         <f t="shared" si="0"/>
-        <v>0.41054550597029604</v>
+        <v>0.56344883657101363</v>
       </c>
       <c r="T3">
         <f t="shared" si="0"/>
-        <v>0.36702768233744465</v>
+        <v>0.52400741801104267</v>
       </c>
       <c r="U3">
         <f t="shared" si="0"/>
-        <v>0.32702166496266316</v>
+        <v>0.48208682457015928</v>
       </c>
       <c r="V3">
         <f t="shared" si="0"/>
-        <v>0.2903952384868449</v>
+        <v>0.44351987860454656</v>
       </c>
       <c r="W3">
         <f t="shared" si="0"/>
-        <v>0.25699978606085772</v>
+        <v>0.40803828831618283</v>
       </c>
       <c r="X3">
         <f t="shared" si="0"/>
-        <v>0.22693081109173738</v>
+        <v>0.37131484236772638</v>
       </c>
       <c r="Y3">
         <f t="shared" si="0"/>
-        <v>0.19969911376072888</v>
+        <v>0.33789650655463099</v>
       </c>
       <c r="Z3">
         <f t="shared" si="0"/>
-        <v>0.17553552099568068</v>
+        <v>0.30748582096471422</v>
       </c>
       <c r="AA3">
         <f t="shared" si="0"/>
-        <v>0.15394465191321197</v>
+        <v>0.27673723886824281</v>
       </c>
       <c r="AB3">
         <f t="shared" si="0"/>
-        <v>0.13470157042406047</v>
+        <v>0.24906351498141854</v>
       </c>
       <c r="AC3">
         <f t="shared" si="0"/>
-        <v>0.11786387412105291</v>
+        <v>0.22415716348327669</v>
       </c>
       <c r="AD3">
         <f t="shared" si="0"/>
-        <v>0.1028951621076792</v>
+        <v>0.19949987550011625</v>
       </c>
       <c r="AE3">
         <f t="shared" si="0"/>
-        <v>8.9724581357896266E-2</v>
+        <v>0.17755488919510345</v>
       </c>
       <c r="AF3">
         <f t="shared" si="0"/>
-        <v>2.6917374407368879E-2</v>
+        <v>5.3266466758531035E-2</v>
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.3">
@@ -7913,203 +7923,203 @@
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>0.99739212515354392</v>
+        <v>0.99831675588711721</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>0.98924478377020841</v>
+        <v>0.99299980499619667</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>0.97547709475632682</v>
+        <v>0.98393537137827769</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>0.95620855917354664</v>
+        <v>0.97113236564271588</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>0.9316924007853824</v>
+        <v>0.95467296316352146</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
-        <v>0.9022923362809403</v>
+        <v>0.93469856026807085</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>0.86846519465567973</v>
+        <v>0.911401681881576</v>
       </c>
       <c r="J4">
         <f t="shared" si="1"/>
-        <v>0.83074410220315842</v>
+        <v>0.88501939607412372</v>
       </c>
       <c r="K4">
         <f t="shared" si="1"/>
-        <v>0.78972109891259246</v>
+        <v>0.85582699409730667</v>
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>0.74602916969698607</v>
+        <v>0.82413154571082692</v>
       </c>
       <c r="M4">
         <f t="shared" si="1"/>
-        <v>0.7003240706390983</v>
+        <v>0.79026524479839177</v>
       </c>
       <c r="N4">
         <f t="shared" si="1"/>
-        <v>0.653266479136134</v>
+        <v>0.75457859105805325</v>
       </c>
       <c r="O4">
         <f t="shared" si="1"/>
-        <v>0.60550503200212358</v>
+        <v>0.71743351493239338</v>
       </c>
       <c r="P4">
         <f t="shared" si="1"/>
-        <v>0.55766078616588688</v>
+        <v>0.67919658109746339</v>
       </c>
       <c r="Q4">
         <f t="shared" si="1"/>
-        <v>0.51031356554733853</v>
+        <v>0.64023241524371066</v>
       </c>
       <c r="R4">
         <f t="shared" si="1"/>
-        <v>0.46399055920833854</v>
+        <v>0.60089749623889543</v>
       </c>
       <c r="S4">
         <f t="shared" si="1"/>
-        <v>0.41915742089838504</v>
+        <v>0.56153444467433955</v>
       </c>
       <c r="T4">
         <f t="shared" si="1"/>
-        <v>0.37621199808238615</v>
+        <v>0.52246692159518826</v>
       </c>
       <c r="U4">
         <f t="shared" si="1"/>
-        <v>0.33548069779147327</v>
+        <v>0.48399522967902553</v>
       </c>
       <c r="V4">
         <f t="shared" si="1"/>
-        <v>0.2972173843787802</v>
+        <v>0.44639268476921745</v>
       </c>
       <c r="W4">
         <f t="shared" si="1"/>
-        <v>0.26160460635360461</v>
+        <v>0.4099027998534206</v>
       </c>
       <c r="X4">
         <f t="shared" si="1"/>
-        <v>0.22875687025273661</v>
+        <v>0.37473729754723328</v>
       </c>
       <c r="Y4">
         <f t="shared" si="1"/>
-        <v>0.1987256217057094</v>
+        <v>0.34107494201536037</v>
       </c>
       <c r="Z4">
         <f t="shared" si="1"/>
-        <v>0.1715055585548676</v>
+        <v>0.30906115800942446</v>
       </c>
       <c r="AA4">
         <f t="shared" si="1"/>
-        <v>0.14704188767634285</v>
+        <v>0.27880838412656883</v>
       </c>
       <c r="AB4">
         <f t="shared" si="1"/>
-        <v>0.12523814427017732</v>
+        <v>0.25039709011459887</v>
       </c>
       <c r="AC4">
         <f t="shared" si="1"/>
-        <v>0.10596421705503067</v>
+        <v>0.22387737448999978</v>
       </c>
       <c r="AD4">
         <f t="shared" si="1"/>
-        <v>8.9064261489625096E-2</v>
+        <v>0.19927104911966265</v>
       </c>
       <c r="AE4">
         <f t="shared" si="1"/>
-        <v>7.4364231919015422E-2</v>
+        <v>0.17657411178033777</v>
       </c>
       <c r="AF4">
         <f t="shared" si="1"/>
-        <v>6.1678818389612644E-2</v>
+        <v>0.15575950591235288</v>
       </c>
       <c r="AG4">
         <f t="shared" ref="AG4:AZ4" si="2">1-_xlfn.WEIBULL.DIST(AG1,$B$10,$B$12,TRUE)</f>
-        <v>5.0817630964475224E-2</v>
+        <v>0.13678006853521585</v>
       </c>
       <c r="AH4">
         <f t="shared" si="2"/>
-        <v>4.1590530289999483E-2</v>
+        <v>0.1195715721785825</v>
       </c>
       <c r="AI4">
         <f t="shared" si="2"/>
-        <v>3.3812055089708859E-2</v>
+        <v>0.10405577419740442</v>
       </c>
       <c r="AJ4">
         <f t="shared" si="2"/>
-        <v>2.7304943043493068E-2</v>
+        <v>9.0143396421134003E-2</v>
       </c>
       <c r="AK4">
         <f t="shared" si="2"/>
-        <v>2.1902779718167675E-2</v>
+        <v>7.773696914395567E-2</v>
       </c>
       <c r="AL4">
         <f t="shared" si="2"/>
-        <v>1.7451840104900196E-2</v>
+        <v>6.6733485410649274E-2</v>
       </c>
       <c r="AM4">
         <f t="shared" si="2"/>
-        <v>1.3812208770020096E-2</v>
+        <v>5.7026823836338725E-2</v>
       </c>
       <c r="AN4">
         <f t="shared" si="2"/>
-        <v>1.085827803774464E-2</v>
+        <v>4.8509910316327787E-2</v>
       </c>
       <c r="AO4">
         <f t="shared" si="2"/>
-        <v>8.4787297965790431E-3</v>
+        <v>4.1076600502268801E-2</v>
       </c>
       <c r="AP4">
         <f t="shared" si="2"/>
-        <v>6.5761065295036891E-3</v>
+        <v>3.4623275491463823E-2</v>
       </c>
       <c r="AQ4">
         <f t="shared" si="2"/>
-        <v>5.0660722372383171E-3</v>
+        <v>2.9050152531782669E-2</v>
       </c>
       <c r="AR4">
         <f t="shared" si="2"/>
-        <v>3.8764553222113696E-3</v>
+        <v>2.4262320506897139E-2</v>
       </c>
       <c r="AS4">
         <f t="shared" si="2"/>
-        <v>2.9461544491962144E-3</v>
+        <v>2.0170516439616759E-2</v>
       </c>
       <c r="AT4">
         <f t="shared" si="2"/>
-        <v>2.2239760017190857E-3</v>
+        <v>1.6691664214857793E-2</v>
       </c>
       <c r="AU4">
         <f t="shared" si="2"/>
-        <v>1.6674589543207441E-3</v>
+        <v>1.3749200223324487E-2</v>
       </c>
       <c r="AV4">
         <f t="shared" si="2"/>
-        <v>1.2417305360230557E-3</v>
+        <v>1.1273212760904316E-2</v>
       </c>
       <c r="AW4">
         <f t="shared" si="2"/>
-        <v>9.1842453361701271E-4</v>
+        <v>9.2004229263573656E-3</v>
       </c>
       <c r="AX4">
         <f t="shared" si="2"/>
-        <v>6.7468385411284526E-4</v>
+        <v>7.47403460837337E-3</v>
       </c>
       <c r="AY4">
         <f t="shared" si="2"/>
-        <v>4.9226024838955329E-4</v>
+        <v>6.0434801255350168E-3</v>
       </c>
       <c r="AZ4">
         <f t="shared" si="2"/>
-        <v>3.5671696845152034E-4</v>
+        <v>4.8640863672232415E-3</v>
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.3">
@@ -8122,199 +8132,199 @@
       </c>
       <c r="C5">
         <f t="shared" ref="C5" si="4">C4-(C1/$AZ$1)*$AZ$4</f>
-        <v>0.99738499081417487</v>
+        <v>0.99821947415977275</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5" si="5">D4-(D1/$AZ$1)*$AZ$4</f>
-        <v>0.98923051509147031</v>
+        <v>0.99280524154150773</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5" si="6">E4-(E1/$AZ$1)*$AZ$4</f>
-        <v>0.97545569173821978</v>
+        <v>0.98364352619624429</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5" si="7">F4-(F1/$AZ$1)*$AZ$4</f>
-        <v>0.95618002181607054</v>
+        <v>0.97074323873333801</v>
       </c>
       <c r="G5">
         <f t="shared" ref="G5" si="8">G4-(G1/$AZ$1)*$AZ$4</f>
-        <v>0.93165672908853725</v>
+        <v>0.95418655452679912</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5" si="9">H4-(H1/$AZ$1)*$AZ$4</f>
-        <v>0.90224953024472609</v>
+        <v>0.93411486990400405</v>
       </c>
       <c r="I5">
         <f t="shared" ref="I5" si="10">I4-(I1/$AZ$1)*$AZ$4</f>
-        <v>0.86841525428009647</v>
+        <v>0.91072070979016473</v>
       </c>
       <c r="J5">
         <f t="shared" ref="J5" si="11">J4-(J1/$AZ$1)*$AZ$4</f>
-        <v>0.83068702748820622</v>
+        <v>0.88424114225536798</v>
       </c>
       <c r="K5">
         <f t="shared" ref="K5" si="12">K4-(K1/$AZ$1)*$AZ$4</f>
-        <v>0.7896568898582712</v>
+        <v>0.85495145855120647</v>
       </c>
       <c r="L5">
         <f t="shared" ref="L5" si="13">L4-(L1/$AZ$1)*$AZ$4</f>
-        <v>0.74595782630329577</v>
+        <v>0.82315872843738225</v>
       </c>
       <c r="M5">
         <f t="shared" ref="M5" si="14">M4-(M1/$AZ$1)*$AZ$4</f>
-        <v>0.70024559290603894</v>
+        <v>0.78919514579760264</v>
       </c>
       <c r="N5">
         <f t="shared" ref="N5" si="15">N4-(N1/$AZ$1)*$AZ$4</f>
-        <v>0.65318086706370559</v>
+        <v>0.75341121032991965</v>
       </c>
       <c r="O5">
         <f t="shared" ref="O5" si="16">O4-(O1/$AZ$1)*$AZ$4</f>
-        <v>0.60541228559032623</v>
+        <v>0.71616885247691531</v>
       </c>
       <c r="P5">
         <f t="shared" ref="P5" si="17">P4-(P1/$AZ$1)*$AZ$4</f>
-        <v>0.55756090541472048</v>
+        <v>0.67783463691464085</v>
       </c>
       <c r="Q5">
         <f t="shared" ref="Q5" si="18">Q4-(Q1/$AZ$1)*$AZ$4</f>
-        <v>0.51020655045680308</v>
+        <v>0.63877318933354366</v>
       </c>
       <c r="R5">
         <f t="shared" ref="R5" si="19">R4-(R1/$AZ$1)*$AZ$4</f>
-        <v>0.46387640977843403</v>
+        <v>0.59934098860138396</v>
       </c>
       <c r="S5">
         <f t="shared" ref="S5" si="20">S4-(S1/$AZ$1)*$AZ$4</f>
-        <v>0.41903613712911153</v>
+        <v>0.55988065530948361</v>
       </c>
       <c r="T5">
         <f t="shared" ref="T5" si="21">T4-(T1/$AZ$1)*$AZ$4</f>
-        <v>0.37608357997374359</v>
+        <v>0.52071585050298785</v>
       </c>
       <c r="U5">
         <f t="shared" ref="U5" si="22">U4-(U1/$AZ$1)*$AZ$4</f>
-        <v>0.33534514534346171</v>
+        <v>0.48214687685948071</v>
       </c>
       <c r="V5">
         <f t="shared" ref="V5" si="23">V4-(V1/$AZ$1)*$AZ$4</f>
-        <v>0.29707469759139959</v>
+        <v>0.44444705022232817</v>
       </c>
       <c r="W5">
         <f t="shared" ref="W5" si="24">W4-(W1/$AZ$1)*$AZ$4</f>
-        <v>0.26145478522685495</v>
+        <v>0.40785988357918684</v>
       </c>
       <c r="X5">
         <f t="shared" ref="X5" si="25">X4-(X1/$AZ$1)*$AZ$4</f>
-        <v>0.22859991478661795</v>
+        <v>0.37259709954565506</v>
       </c>
       <c r="Y5">
         <f t="shared" ref="Y5" si="26">Y4-(Y1/$AZ$1)*$AZ$4</f>
-        <v>0.19856153190022169</v>
+        <v>0.33883746228643769</v>
       </c>
       <c r="Z5">
         <f t="shared" ref="Z5" si="27">Z4-(Z1/$AZ$1)*$AZ$4</f>
-        <v>0.17133433441001086</v>
+        <v>0.30672639655315731</v>
       </c>
       <c r="AA5">
         <f t="shared" ref="AA5" si="28">AA4-(AA1/$AZ$1)*$AZ$4</f>
-        <v>0.14686352919211709</v>
+        <v>0.27637634094295721</v>
       </c>
       <c r="AB5">
         <f t="shared" ref="AB5" si="29">AB4-(AB1/$AZ$1)*$AZ$4</f>
-        <v>0.12505265144658254</v>
+        <v>0.24786776520364279</v>
       </c>
       <c r="AC5">
         <f t="shared" ref="AC5" si="30">AC4-(AC1/$AZ$1)*$AZ$4</f>
-        <v>0.10577158989206685</v>
+        <v>0.22125076785169923</v>
       </c>
       <c r="AD5">
         <f t="shared" ref="AD5" si="31">AD4-(AD1/$AZ$1)*$AZ$4</f>
-        <v>8.8864499987292248E-2</v>
+        <v>0.19654716075401762</v>
       </c>
       <c r="AE5">
         <f t="shared" ref="AE5" si="32">AE4-(AE1/$AZ$1)*$AZ$4</f>
-        <v>7.4157336077313535E-2</v>
+        <v>0.17375294168734828</v>
       </c>
       <c r="AF5">
         <f t="shared" ref="AF5" si="33">AF4-(AF1/$AZ$1)*$AZ$4</f>
-        <v>6.1464788208541732E-2</v>
+        <v>0.15284105409201892</v>
       </c>
       <c r="AG5">
         <f t="shared" ref="AG5:AY5" si="34">AG4-(AG1/$AZ$1)*$AZ$4</f>
-        <v>5.059646644403528E-2</v>
+        <v>0.13376433498753743</v>
       </c>
       <c r="AH5">
         <f t="shared" si="34"/>
-        <v>4.1362231430190508E-2</v>
+        <v>0.11645855690355962</v>
       </c>
       <c r="AI5">
         <f t="shared" si="34"/>
-        <v>3.3576621890530858E-2</v>
+        <v>0.10084547719503707</v>
       </c>
       <c r="AJ5">
         <f t="shared" si="34"/>
-        <v>2.7062375504946036E-2</v>
+        <v>8.6835817691422193E-2</v>
       </c>
       <c r="AK5">
         <f t="shared" si="34"/>
-        <v>2.1653077840251611E-2</v>
+        <v>7.4332108686899406E-2</v>
       </c>
       <c r="AL5">
         <f t="shared" si="34"/>
-        <v>1.71950038876151E-2</v>
+        <v>6.3231343226248543E-2</v>
       </c>
       <c r="AM5">
         <f t="shared" si="34"/>
-        <v>1.3548238213365971E-2</v>
+        <v>5.3427399924593527E-2</v>
       </c>
       <c r="AN5">
         <f t="shared" si="34"/>
-        <v>1.0587173141721484E-2</v>
+        <v>4.4813204677238122E-2</v>
       </c>
       <c r="AO5">
         <f t="shared" si="34"/>
-        <v>8.2004905611868569E-3</v>
+        <v>3.7282613135834669E-2</v>
       </c>
       <c r="AP5">
         <f t="shared" si="34"/>
-        <v>6.2907329547424728E-3</v>
+        <v>3.0732006397685231E-2</v>
       </c>
       <c r="AQ5">
         <f t="shared" si="34"/>
-        <v>4.7735643231080708E-3</v>
+        <v>2.506160171065961E-2</v>
       </c>
       <c r="AR5">
         <f t="shared" si="34"/>
-        <v>3.5768130687120923E-3</v>
+        <v>2.0176487958429617E-2</v>
       </c>
       <c r="AS5">
         <f t="shared" si="34"/>
-        <v>2.6393778563279071E-3</v>
+        <v>1.5987402163804773E-2</v>
       </c>
       <c r="AT5">
         <f t="shared" si="34"/>
-        <v>1.9100650694817479E-3</v>
+        <v>1.241126821170134E-2</v>
       </c>
       <c r="AU5">
         <f t="shared" si="34"/>
-        <v>1.3464136827143758E-3</v>
+        <v>9.3715224928235703E-3</v>
       </c>
       <c r="AV5">
         <f t="shared" si="34"/>
-        <v>9.1355092504765692E-4</v>
+        <v>6.7982533030589345E-3</v>
       </c>
       <c r="AW5">
         <f t="shared" si="34"/>
-        <v>5.8311058327258363E-4</v>
+        <v>4.6281817411675192E-3</v>
       </c>
       <c r="AX5">
         <f t="shared" si="34"/>
-        <v>3.3223556439938574E-4</v>
+        <v>2.8045116958390582E-3</v>
       </c>
       <c r="AY5">
         <f t="shared" si="34"/>
-        <v>1.4267761930706339E-4</v>
+        <v>1.2766754856562406E-3</v>
       </c>
       <c r="AZ5">
         <v>0</v>
@@ -8322,207 +8332,207 @@
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B6">
         <f>B5/SUM($B$5:$AZ$5)</f>
-        <v>6.0192694283551618E-2</v>
+        <v>4.9941081907415655E-2</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:AZ6" si="35">C5/SUM($B$5:$AZ$5)</f>
-        <v>6.0035289835080566E-2</v>
+        <v>4.9852160520590598E-2</v>
       </c>
       <c r="D6">
         <f t="shared" si="35"/>
-        <v>5.9544449970861169E-2</v>
+        <v>4.9581767885936025E-2</v>
       </c>
       <c r="E6">
         <f t="shared" si="35"/>
-        <v>5.8715306239949035E-2</v>
+        <v>4.9124221909465797E-2</v>
       </c>
       <c r="F6">
         <f t="shared" si="35"/>
-        <v>5.755505173321445E-2</v>
+        <v>4.8479967596651581E-2</v>
       </c>
       <c r="G6">
         <f t="shared" si="35"/>
-        <v>5.6078928671239994E-2</v>
+        <v>4.7653108874577611E-2</v>
       </c>
       <c r="H6">
         <f t="shared" si="35"/>
-        <v>5.4308830141498857E-2</v>
+        <v>4.6650707228810789E-2</v>
       </c>
       <c r="I6">
         <f t="shared" si="35"/>
-        <v>5.2272253912054589E-2</v>
+        <v>4.5482377562410338E-2</v>
       </c>
       <c r="J6">
         <f t="shared" si="35"/>
-        <v>5.0001290290909842E-2</v>
+        <v>4.415995931128211E-2</v>
       </c>
       <c r="K6">
         <f t="shared" si="35"/>
-        <v>4.7531575760139111E-2</v>
+        <v>4.2697200818370286E-2</v>
       </c>
       <c r="L6">
         <f t="shared" si="35"/>
-        <v>4.4901211387096983E-2</v>
+        <v>4.1109437479695428E-2</v>
       </c>
       <c r="M6">
         <f t="shared" si="35"/>
-        <v>4.2149668897197547E-2</v>
+        <v>3.9413259417212916E-2</v>
       </c>
       <c r="N6">
         <f t="shared" si="35"/>
-        <v>3.9316716243030805E-2</v>
+        <v>3.7626170965051685E-2</v>
       </c>
       <c r="O6">
         <f t="shared" si="35"/>
-        <v>3.644139662204475E-2</v>
+        <v>3.576624732108951E-2</v>
       </c>
       <c r="P6">
         <f t="shared" si="35"/>
-        <v>3.356109312408851E-2</v>
+        <v>3.3851795121837433E-2</v>
       </c>
       <c r="Q6">
         <f t="shared" si="35"/>
-        <v>3.0710706913111802E-2</v>
+        <v>3.1901024168767632E-2</v>
       </c>
       <c r="R6">
         <f t="shared" si="35"/>
-        <v>2.7921970919144796E-2</v>
+        <v>2.993173740221319E-2</v>
       </c>
       <c r="S6">
         <f t="shared" si="35"/>
-        <v>2.5222914095973024E-2</v>
+        <v>2.7961045665188474E-2</v>
       </c>
       <c r="T6">
         <f t="shared" si="35"/>
-        <v>2.2637483954423183E-2</v>
+        <v>2.6005112940459322E-2</v>
       </c>
       <c r="U6">
         <f t="shared" si="35"/>
-        <v>2.0185327813132176E-2</v>
+        <v>2.4078936668643976E-2</v>
       </c>
       <c r="V6">
         <f t="shared" si="35"/>
-        <v>1.7881726451497666E-2</v>
+        <v>2.2196166538662569E-2</v>
       </c>
       <c r="W6">
         <f t="shared" si="35"/>
-        <v>1.573766795613173E-2</v>
+        <v>2.0368963852577183E-2</v>
       </c>
       <c r="X6">
         <f t="shared" si="35"/>
-        <v>1.3760044783996846E-2</v>
+        <v>1.8607902266875063E-2</v>
       </c>
       <c r="Y6">
         <f t="shared" si="35"/>
-        <v>1.1951953586143727E-2</v>
+        <v>1.6921909457347849E-2</v>
       </c>
       <c r="Z6">
         <f t="shared" si="35"/>
-        <v>1.0313075211417583E-2</v>
+        <v>1.5318248093427685E-2</v>
       </c>
       <c r="AA6">
         <f t="shared" si="35"/>
-        <v>8.8401115140645629E-3</v>
+        <v>1.3802533480304061E-2</v>
       </c>
       <c r="AB6">
         <f t="shared" si="35"/>
-        <v>7.527256017871682E-3</v>
+        <v>1.2378784364243197E-2</v>
       </c>
       <c r="AC6">
         <f t="shared" si="35"/>
-        <v>6.3666769742583788E-3</v>
+        <v>1.1049502719360317E-2</v>
       </c>
       <c r="AD6">
         <f t="shared" si="35"/>
-        <v>5.3489936803957595E-3</v>
+        <v>9.8157778538863864E-3</v>
       </c>
       <c r="AE6">
         <f t="shared" si="35"/>
-        <v>4.4637298593843263E-3</v>
+        <v>8.6774098924622765E-3</v>
       </c>
       <c r="AF6">
         <f t="shared" si="35"/>
-        <v>3.6997312058400008E-3</v>
+        <v>7.6330476012252636E-3</v>
       </c>
       <c r="AG6">
         <f t="shared" si="35"/>
-        <v>3.0455376364937939E-3</v>
+        <v>6.680335609903592E-3</v>
       </c>
       <c r="AH6">
         <f t="shared" si="35"/>
-        <v>2.4897041513629674E-3</v>
+        <v>5.8160663291400979E-3</v>
       </c>
       <c r="AI6">
         <f t="shared" si="35"/>
-        <v>2.0210673365311312E-3</v>
+        <v>5.0363322365897644E-3</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="35"/>
-        <v>1.6289572953558926E-3</v>
+        <v>4.336674683824729E-3</v>
       </c>
       <c r="AK6">
         <f t="shared" si="35"/>
-        <v>1.3033570947362115E-3</v>
+        <v>3.712225928283366E-3</v>
       </c>
       <c r="AL6">
         <f t="shared" si="35"/>
-        <v>1.0350136122116973E-3</v>
+        <v>3.1578416911779905E-3</v>
       </c>
       <c r="AM6">
         <f t="shared" si="35"/>
-        <v>8.155049608578695E-4</v>
+        <v>2.6682221557343786E-3</v>
       </c>
       <c r="AN6">
         <f t="shared" si="35"/>
-        <v>6.3727047624667003E-4</v>
+        <v>2.2380199253197314E-3</v>
       </c>
       <c r="AO6">
         <f t="shared" si="35"/>
-        <v>4.9360962132467118E-4</v>
+        <v>1.8619340363392101E-3</v>
       </c>
       <c r="AP6">
         <f t="shared" si="35"/>
-        <v>3.7865616556427702E-4</v>
+        <v>1.53478964868602E-3</v>
       </c>
       <c r="AQ6">
         <f t="shared" si="35"/>
-        <v>2.8733369794371315E-4</v>
+        <v>1.2516035037630799E-3</v>
       </c>
       <c r="AR6">
         <f t="shared" si="35"/>
-        <v>2.1529801555439907E-4</v>
+        <v>1.0076356377359192E-3</v>
       </c>
       <c r="AS6">
         <f t="shared" si="35"/>
-        <v>1.5887126440472155E-4</v>
+        <v>7.9842816094936842E-4</v>
       </c>
       <c r="AT6">
         <f t="shared" si="35"/>
-        <v>1.1497196278900563E-4</v>
+        <v>6.1983216233548084E-4</v>
       </c>
       <c r="AU6">
         <f t="shared" si="35"/>
-        <v>8.1044267182817299E-5</v>
+        <v>4.6802397241129008E-4</v>
       </c>
       <c r="AV6">
         <f t="shared" si="35"/>
-        <v>5.4989091543849397E-5</v>
+        <v>3.395121250354253E-4</v>
       </c>
       <c r="AW6">
         <f t="shared" si="35"/>
-        <v>3.5098997072430095E-5</v>
+        <v>2.3113640341805268E-4</v>
       </c>
       <c r="AX6">
         <f t="shared" si="35"/>
-        <v>1.9998153758015452E-5</v>
+        <v>1.4006034831220358E-4</v>
       </c>
       <c r="AY6">
         <f t="shared" si="35"/>
-        <v>8.5881503200550279E-6</v>
+        <v>6.3758554998347974E-5</v>
       </c>
       <c r="AZ6">
         <f t="shared" si="35"/>
@@ -8531,206 +8541,206 @@
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
         <f>(B5-C5)/B5</f>
-        <v>2.6150091858251345E-3</v>
+        <v>1.7805258402272539E-3</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:AZ7" si="36">(C5-D5)/C5</f>
-        <v>8.1758556603583749E-3</v>
+        <v>5.4238899945548685E-3</v>
       </c>
       <c r="E7">
         <f t="shared" si="36"/>
-        <v>1.3924786127303026E-2</v>
+        <v>9.2281093631599309E-3</v>
       </c>
       <c r="F7">
         <f t="shared" si="36"/>
-        <v>1.9760682197466944E-2</v>
+        <v>1.3114799334665243E-2</v>
       </c>
       <c r="G7">
         <f t="shared" si="36"/>
-        <v>2.5647150293891575E-2</v>
+        <v>1.7055678109221407E-2</v>
       </c>
       <c r="H7">
         <f t="shared" si="36"/>
-        <v>3.1564414151316167E-2</v>
+        <v>2.1035388234692781E-2</v>
       </c>
       <c r="I7">
         <f t="shared" si="36"/>
-        <v>3.7499909759390417E-2</v>
+        <v>2.5044200523478943E-2</v>
       </c>
       <c r="J7">
         <f t="shared" si="36"/>
-        <v>4.3444914867561142E-2</v>
+        <v>2.9075398473037677E-2</v>
       </c>
       <c r="K7">
         <f t="shared" si="36"/>
-        <v>4.939301598822373E-2</v>
+        <v>3.3124090595303565E-2</v>
       </c>
       <c r="L7">
         <f t="shared" si="36"/>
-        <v>5.533930510353504E-2</v>
+        <v>3.7186590882832007E-2</v>
       </c>
       <c r="M7">
         <f t="shared" si="36"/>
-        <v>6.1279916619134567E-2</v>
+        <v>4.1260064998950227E-2</v>
       </c>
       <c r="N7">
         <f t="shared" si="36"/>
-        <v>6.7211741593422109E-2</v>
+        <v>4.5342315722834106E-2</v>
       </c>
       <c r="O7">
         <f t="shared" si="36"/>
-        <v>7.3132242357491523E-2</v>
+        <v>4.943164813899685E-2</v>
       </c>
       <c r="P7">
         <f t="shared" si="36"/>
-        <v>7.9039327933272382E-2</v>
+        <v>5.3526784123175901E-2</v>
       </c>
       <c r="Q7">
         <f t="shared" si="36"/>
-        <v>8.4931268491098139E-2</v>
+        <v>5.7626809628520313E-2</v>
       </c>
       <c r="R7">
         <f t="shared" si="36"/>
-        <v>9.0806636325794512E-2</v>
+        <v>6.1731145562481743E-2</v>
       </c>
       <c r="S7">
         <f t="shared" si="36"/>
-        <v>9.6664265964160612E-2</v>
+        <v>6.5839537162283163E-2</v>
       </c>
       <c r="T7">
         <f t="shared" si="36"/>
-        <v>0.10250322907623978</v>
+        <v>6.9952059309580428E-2</v>
       </c>
       <c r="U7">
         <f t="shared" si="36"/>
-        <v>0.10832282183956567</v>
+        <v>7.4069136951086217E-2</v>
       </c>
       <c r="V7">
         <f t="shared" si="36"/>
-        <v>0.11412256382261145</v>
+        <v>7.8191581127134355E-2</v>
       </c>
       <c r="W7">
         <f t="shared" si="36"/>
-        <v>0.11990220861399896</v>
+        <v>8.2320642301122543E-2</v>
       </c>
       <c r="X7">
         <f t="shared" si="36"/>
-        <v>0.12566176752791119</v>
+        <v>8.6458083899014881E-2</v>
       </c>
       <c r="Y7">
         <f t="shared" si="36"/>
-        <v>0.13140154892198885</v>
+        <v>9.0606280350501611E-2</v>
       </c>
       <c r="Z7">
         <f t="shared" si="36"/>
-        <v>0.13712221712659151</v>
+        <v>9.4768345615028685E-2</v>
       </c>
       <c r="AA7">
         <f t="shared" si="36"/>
-        <v>0.14282487688272696</v>
+        <v>9.8948300346039089E-2</v>
       </c>
       <c r="AB7">
         <f t="shared" si="36"/>
-        <v>0.14851119175410132</v>
+        <v>0.10315128871757681</v>
       </c>
       <c r="AC7">
         <f t="shared" si="36"/>
-        <v>0.15418354854116612</v>
+        <v>0.10738385981765565</v>
       </c>
       <c r="AD7">
         <f t="shared" si="36"/>
-        <v>0.1598452847501603</v>
+        <v>0.11165433384728421</v>
       </c>
       <c r="AE7">
         <f t="shared" si="36"/>
-        <v>0.1655010033487147</v>
+        <v>0.11597328081068911</v>
       </c>
       <c r="AF7">
         <f t="shared" si="36"/>
-        <v>0.17115700940954851</v>
+        <v>0.12035414993409603</v>
       </c>
       <c r="AG7">
         <f t="shared" si="36"/>
-        <v>0.17682191839060279</v>
+        <v>0.1248141032382323</v>
       </c>
       <c r="AH7">
         <f t="shared" si="36"/>
-        <v>0.18250750818851658</v>
+        <v>0.12937512892050151</v>
       </c>
       <c r="AI7">
         <f t="shared" si="36"/>
-        <v>0.18822992064148872</v>
+        <v>0.13406554334562018</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="36"/>
-        <v>0.19401136918487752</v>
+        <v>0.13892204086178234</v>
       </c>
       <c r="AK7">
         <f t="shared" si="36"/>
-        <v>0.1998825884189582</v>
+        <v>0.14399252908466512</v>
       </c>
       <c r="AL7">
         <f t="shared" si="36"/>
-        <v>0.2058863864770879</v>
+        <v>0.14934011232493538</v>
       </c>
       <c r="AM7">
         <f t="shared" si="36"/>
-        <v>0.2120828641903218</v>
+        <v>0.15504879070140029</v>
       </c>
       <c r="AN7">
         <f t="shared" si="36"/>
-        <v>0.21855720463515754</v>
+        <v>0.16123178854882186</v>
       </c>
       <c r="AO7">
         <f t="shared" si="36"/>
-        <v>0.22543152441035361</v>
+        <v>0.16804403067447776</v>
       </c>
       <c r="AP7">
         <f t="shared" si="36"/>
-        <v>0.23288333694124572</v>
+        <v>0.17570138429629648</v>
       </c>
       <c r="AQ7">
         <f t="shared" si="36"/>
-        <v>0.24117517665260854</v>
+        <v>0.184511372724845</v>
       </c>
       <c r="AR7">
         <f t="shared" si="36"/>
-        <v>0.25070391292366057</v>
+        <v>0.19492424341546283</v>
       </c>
       <c r="AS7">
         <f t="shared" si="36"/>
-        <v>0.26208672199962879</v>
+        <v>0.20762214926878136</v>
       </c>
       <c r="AT7">
         <f t="shared" si="36"/>
-        <v>0.27631996119753455</v>
+        <v>0.22368449329433546</v>
       </c>
       <c r="AU7">
         <f t="shared" si="36"/>
-        <v>0.29509538485005954</v>
+        <v>0.244918220042324</v>
       </c>
       <c r="AV7">
         <f t="shared" si="36"/>
-        <v>0.32149313633984</v>
+        <v>0.27458389943951667</v>
       </c>
       <c r="AW7">
         <f t="shared" si="36"/>
-        <v>0.36170982122078776</v>
+        <v>0.31921016548691594</v>
       </c>
       <c r="AX7">
         <f t="shared" si="36"/>
-        <v>0.43023574956437149</v>
+        <v>0.39403596213756642</v>
       </c>
       <c r="AY7">
         <f t="shared" si="36"/>
-        <v>0.57055284082847824</v>
+        <v>0.54477797773124181</v>
       </c>
       <c r="AZ7">
         <f t="shared" si="36"/>
@@ -8748,15 +8758,22 @@
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B10" s="16">
-        <v>2.0499999999999998</v>
-      </c>
+        <v>2.06</v>
+      </c>
+      <c r="AS10" s="22"/>
+      <c r="AT10" s="22"/>
+      <c r="AU10" s="22"/>
+      <c r="AV10" s="22"/>
+      <c r="AW10" s="22"/>
+      <c r="AX10" s="22"/>
+      <c r="AY10" s="22"/>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>13</v>
@@ -8764,10 +8781,10 @@
     </row>
     <row r="12" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B12" s="19">
-        <v>18.2</v>
+        <v>22.2</v>
       </c>
     </row>
   </sheetData>
@@ -9371,642 +9388,642 @@
   <sheetData>
     <row r="1" spans="1:211" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AH1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AI1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AK1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AL1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AM1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AN1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AO1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AP1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AR1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AQ1" s="8" t="s">
+      <c r="AS1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AT1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="AS1" s="8" t="s">
+      <c r="AU1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AV1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="AU1" s="8" t="s">
+      <c r="AW1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="AV1" s="8" t="s">
+      <c r="AX1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AW1" s="8" t="s">
+      <c r="AY1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="AX1" s="8" t="s">
+      <c r="AZ1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="AY1" s="8" t="s">
+      <c r="BA1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="AZ1" s="8" t="s">
+      <c r="BB1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="BA1" s="8" t="s">
+      <c r="BC1" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="BB1" s="8" t="s">
+      <c r="BD1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="BC1" s="8" t="s">
+      <c r="BE1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="BD1" s="8" t="s">
+      <c r="BF1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="BE1" s="8" t="s">
+      <c r="BG1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="BF1" s="8" t="s">
+      <c r="BH1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="BG1" s="8" t="s">
+      <c r="BI1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="BH1" s="8" t="s">
+      <c r="BJ1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="BI1" s="8" t="s">
+      <c r="BK1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="BJ1" s="8" t="s">
+      <c r="BL1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="BK1" s="8" t="s">
+      <c r="BM1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="BL1" s="8" t="s">
+      <c r="BN1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="BM1" s="8" t="s">
+      <c r="BO1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="BN1" s="8" t="s">
+      <c r="BP1" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="BO1" s="8" t="s">
+      <c r="BQ1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="BP1" s="8" t="s">
+      <c r="BR1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="BQ1" s="8" t="s">
+      <c r="BS1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="BR1" s="8" t="s">
+      <c r="BT1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="BS1" s="8" t="s">
+      <c r="BU1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="BT1" s="8" t="s">
+      <c r="BV1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="BU1" s="8" t="s">
+      <c r="BW1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="BV1" s="8" t="s">
+      <c r="BX1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="BW1" s="8" t="s">
+      <c r="BY1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="BX1" s="8" t="s">
+      <c r="BZ1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="BY1" s="8" t="s">
+      <c r="CA1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="BZ1" s="8" t="s">
+      <c r="CB1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="CA1" s="8" t="s">
+      <c r="CC1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="CB1" s="8" t="s">
+      <c r="CD1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="CC1" s="8" t="s">
+      <c r="CE1" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="CD1" s="8" t="s">
+      <c r="CF1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="CE1" s="8" t="s">
+      <c r="CG1" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="CF1" s="8" t="s">
+      <c r="CH1" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="CG1" s="8" t="s">
+      <c r="CI1" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="CH1" s="8" t="s">
+      <c r="CJ1" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="CI1" s="8" t="s">
+      <c r="CK1" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="CJ1" s="8" t="s">
+      <c r="CL1" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="CK1" s="8" t="s">
+      <c r="CM1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="CL1" s="8" t="s">
+      <c r="CN1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="CM1" s="8" t="s">
+      <c r="CO1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="CN1" s="8" t="s">
+      <c r="CP1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="CO1" s="8" t="s">
+      <c r="CQ1" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="CP1" s="8" t="s">
+      <c r="CR1" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="CQ1" s="8" t="s">
+      <c r="CS1" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="CR1" s="8" t="s">
+      <c r="CT1" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="CS1" s="8" t="s">
+      <c r="CU1" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="CV1" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="CW1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CX1" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="CW1" s="8" t="s">
+      <c r="CY1" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="CX1" s="8" t="s">
+      <c r="CZ1" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="CY1" s="8" t="s">
+      <c r="DA1" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="CZ1" s="8" t="s">
+      <c r="DB1" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="DA1" s="8" t="s">
+      <c r="DC1" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="DB1" s="8" t="s">
+      <c r="DD1" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="DC1" s="8" t="s">
+      <c r="DE1" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="DD1" s="8" t="s">
+      <c r="DF1" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="DE1" s="8" t="s">
+      <c r="DG1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="DF1" s="8" t="s">
+      <c r="DH1" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="DG1" s="8" t="s">
+      <c r="DI1" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="DH1" s="8" t="s">
+      <c r="DJ1" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="DI1" s="8" t="s">
+      <c r="DK1" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="DJ1" s="8" t="s">
+      <c r="DL1" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="DK1" s="8" t="s">
+      <c r="DM1" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="DL1" s="8" t="s">
+      <c r="DN1" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="DM1" s="8" t="s">
+      <c r="DO1" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="DN1" s="8" t="s">
+      <c r="DP1" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="DO1" s="8" t="s">
+      <c r="DQ1" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="DP1" s="8" t="s">
+      <c r="DR1" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="DQ1" s="8" t="s">
+      <c r="DS1" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="DR1" s="8" t="s">
+      <c r="DT1" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="DS1" s="8" t="s">
+      <c r="DU1" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="DT1" s="8" t="s">
+      <c r="DV1" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="DU1" s="8" t="s">
+      <c r="DW1" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="DV1" s="8" t="s">
+      <c r="DX1" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="DW1" s="8" t="s">
+      <c r="DY1" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="DX1" s="8" t="s">
+      <c r="DZ1" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="DY1" s="8" t="s">
+      <c r="EA1" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="DZ1" s="8" t="s">
+      <c r="EB1" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="EA1" s="8" t="s">
+      <c r="EC1" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="EB1" s="8" t="s">
+      <c r="ED1" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="EC1" s="8" t="s">
+      <c r="EE1" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="ED1" s="8" t="s">
+      <c r="EF1" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="EE1" s="8" t="s">
+      <c r="EG1" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="EF1" s="8" t="s">
+      <c r="EH1" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="EG1" s="8" t="s">
+      <c r="EI1" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="EH1" s="8" t="s">
+      <c r="EJ1" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="EI1" s="8" t="s">
+      <c r="EK1" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="EJ1" s="8" t="s">
+      <c r="EL1" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="EK1" s="8" t="s">
+      <c r="EM1" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="EL1" s="8" t="s">
+      <c r="EN1" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="EM1" s="8" t="s">
+      <c r="EO1" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="EN1" s="8" t="s">
+      <c r="EP1" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="EO1" s="8" t="s">
+      <c r="EQ1" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="EP1" s="8" t="s">
+      <c r="ER1" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="EQ1" s="8" t="s">
+      <c r="ES1" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="ER1" s="8" t="s">
+      <c r="ET1" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="ES1" s="8" t="s">
+      <c r="EU1" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="ET1" s="8" t="s">
+      <c r="EV1" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="EU1" s="8" t="s">
+      <c r="EW1" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="EV1" s="8" t="s">
+      <c r="EX1" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="EW1" s="8" t="s">
+      <c r="EY1" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="EX1" s="8" t="s">
+      <c r="EZ1" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="EY1" s="8" t="s">
+      <c r="FA1" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="EZ1" s="8" t="s">
+      <c r="FB1" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="FA1" s="8" t="s">
+      <c r="FC1" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="FB1" s="8" t="s">
+      <c r="FD1" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="FC1" s="8" t="s">
+      <c r="FE1" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="FD1" s="8" t="s">
+      <c r="FF1" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="FE1" s="8" t="s">
+      <c r="FG1" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="FF1" s="8" t="s">
+      <c r="FH1" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="FG1" s="8" t="s">
+      <c r="FI1" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="FH1" s="8" t="s">
+      <c r="FJ1" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="FI1" s="8" t="s">
+      <c r="FK1" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="FJ1" s="8" t="s">
+      <c r="FL1" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="FK1" s="8" t="s">
+      <c r="FM1" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="FL1" s="8" t="s">
+      <c r="FN1" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="FM1" s="8" t="s">
+      <c r="FO1" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="FN1" s="8" t="s">
+      <c r="FP1" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="FO1" s="8" t="s">
+      <c r="FQ1" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="FP1" s="8" t="s">
+      <c r="FR1" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="FQ1" s="8" t="s">
+      <c r="FS1" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="FR1" s="8" t="s">
+      <c r="FT1" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="FS1" s="8" t="s">
+      <c r="FU1" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="FT1" s="8" t="s">
+      <c r="FV1" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="FU1" s="8" t="s">
+      <c r="FW1" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="FV1" s="8" t="s">
+      <c r="FX1" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="FW1" s="8" t="s">
+      <c r="FY1" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="FX1" s="8" t="s">
+      <c r="FZ1" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="FY1" s="8" t="s">
+      <c r="GA1" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="FZ1" s="8" t="s">
+      <c r="GB1" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="GA1" s="8" t="s">
+      <c r="GC1" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="GB1" s="8" t="s">
+      <c r="GD1" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="GC1" s="8" t="s">
+      <c r="GE1" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="GD1" s="8" t="s">
+      <c r="GF1" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="GE1" s="8" t="s">
+      <c r="GG1" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="GF1" s="8" t="s">
+      <c r="GH1" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="GG1" s="8" t="s">
+      <c r="GI1" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="GH1" s="8" t="s">
+      <c r="GJ1" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="GI1" s="8" t="s">
+      <c r="GK1" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="GJ1" s="8" t="s">
+      <c r="GL1" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="GK1" s="8" t="s">
+      <c r="GM1" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="GL1" s="8" t="s">
+      <c r="GN1" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="GM1" s="8" t="s">
+      <c r="GO1" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="GN1" s="8" t="s">
+      <c r="GP1" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="GO1" s="8" t="s">
+      <c r="GQ1" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="GP1" s="8" t="s">
+      <c r="GR1" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="GQ1" s="8" t="s">
+      <c r="GS1" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="GR1" s="8" t="s">
+      <c r="GT1" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="GS1" s="8" t="s">
+      <c r="GU1" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="GT1" s="8" t="s">
+      <c r="GV1" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="GU1" s="8" t="s">
+      <c r="GW1" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="GV1" s="8" t="s">
+      <c r="GX1" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="GW1" s="8" t="s">
+      <c r="GY1" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="GX1" s="8" t="s">
+      <c r="GZ1" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="GY1" s="8" t="s">
+      <c r="HA1" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="GZ1" s="8" t="s">
+      <c r="HB1" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="HA1" s="8" t="s">
+      <c r="HC1" s="8" t="s">
         <v>233</v>
-      </c>
-      <c r="HB1" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="HC1" s="8" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:211" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -10250,203 +10267,203 @@
       </c>
       <c r="CD2" cm="1">
         <f t="array" ref="CD2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CE2:$HC2,"&gt;0")+1)</f>
-        <v>8.5881503200550279E-6</v>
+        <v>6.3758554998347974E-5</v>
       </c>
       <c r="CE2" cm="1">
         <f t="array" ref="CE2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CF2:$HC2,"&gt;0")+1)</f>
-        <v>1.9998153758015452E-5</v>
+        <v>1.4006034831220358E-4</v>
       </c>
       <c r="CF2" cm="1">
         <f t="array" ref="CF2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CG2:$HC2,"&gt;0")+1)</f>
-        <v>3.5098997072430095E-5</v>
+        <v>2.3113640341805268E-4</v>
       </c>
       <c r="CG2" cm="1">
         <f t="array" ref="CG2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CH2:$HC2,"&gt;0")+1)</f>
-        <v>5.4989091543849397E-5</v>
+        <v>3.395121250354253E-4</v>
       </c>
       <c r="CH2" cm="1">
         <f t="array" ref="CH2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CI2:$HC2,"&gt;0")+1)</f>
-        <v>8.1044267182817299E-5</v>
+        <v>4.6802397241129008E-4</v>
       </c>
       <c r="CI2" cm="1">
         <f t="array" ref="CI2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CJ2:$HC2,"&gt;0")+1)</f>
-        <v>1.1497196278900563E-4</v>
+        <v>6.1983216233548084E-4</v>
       </c>
       <c r="CJ2" cm="1">
         <f t="array" ref="CJ2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CK2:$HC2,"&gt;0")+1)</f>
-        <v>1.5887126440472155E-4</v>
+        <v>7.9842816094936842E-4</v>
       </c>
       <c r="CK2" cm="1">
         <f t="array" ref="CK2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CL2:$HC2,"&gt;0")+1)</f>
-        <v>2.1529801555439907E-4</v>
+        <v>1.0076356377359192E-3</v>
       </c>
       <c r="CL2" cm="1">
         <f t="array" ref="CL2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CM2:$HC2,"&gt;0")+1)</f>
-        <v>2.8733369794371315E-4</v>
+        <v>1.2516035037630799E-3</v>
       </c>
       <c r="CM2" cm="1">
         <f t="array" ref="CM2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CN2:$HC2,"&gt;0")+1)</f>
-        <v>3.7865616556427702E-4</v>
+        <v>1.53478964868602E-3</v>
       </c>
       <c r="CN2" cm="1">
         <f t="array" ref="CN2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CO2:$HC2,"&gt;0")+1)</f>
-        <v>4.9360962132467118E-4</v>
+        <v>1.8619340363392101E-3</v>
       </c>
       <c r="CO2" cm="1">
         <f t="array" ref="CO2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CP2:$HC2,"&gt;0")+1)</f>
-        <v>6.3727047624667003E-4</v>
+        <v>2.2380199253197314E-3</v>
       </c>
       <c r="CP2" cm="1">
         <f t="array" ref="CP2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CQ2:$HC2,"&gt;0")+1)</f>
-        <v>8.155049608578695E-4</v>
+        <v>2.6682221557343786E-3</v>
       </c>
       <c r="CQ2" cm="1">
         <f t="array" ref="CQ2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CR2:$HC2,"&gt;0")+1)</f>
-        <v>1.0350136122116973E-3</v>
+        <v>3.1578416911779905E-3</v>
       </c>
       <c r="CR2" cm="1">
         <f t="array" ref="CR2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CS2:$HC2,"&gt;0")+1)</f>
-        <v>1.3033570947362115E-3</v>
+        <v>3.712225928283366E-3</v>
       </c>
       <c r="CS2" cm="1">
         <f t="array" ref="CS2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CT2:$HC2,"&gt;0")+1)</f>
-        <v>1.6289572953558926E-3</v>
+        <v>4.336674683824729E-3</v>
       </c>
       <c r="CT2" cm="1">
         <f t="array" ref="CT2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CU2:$HC2,"&gt;0")+1)</f>
-        <v>2.0210673365311312E-3</v>
+        <v>5.0363322365897644E-3</v>
       </c>
       <c r="CU2" cm="1">
         <f t="array" ref="CU2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CV2:$HC2,"&gt;0")+1)</f>
-        <v>2.4897041513629674E-3</v>
+        <v>5.8160663291400979E-3</v>
       </c>
       <c r="CV2" cm="1">
         <f t="array" ref="CV2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CW2:$HC2,"&gt;0")+1)</f>
-        <v>3.0455376364937939E-3</v>
+        <v>6.680335609903592E-3</v>
       </c>
       <c r="CW2" cm="1">
         <f t="array" ref="CW2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CX2:$HC2,"&gt;0")+1)</f>
-        <v>3.6997312058400008E-3</v>
+        <v>7.6330476012252636E-3</v>
       </c>
       <c r="CX2" cm="1">
         <f t="array" ref="CX2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CY2:$HC2,"&gt;0")+1)</f>
-        <v>4.4637298593843263E-3</v>
+        <v>8.6774098924622765E-3</v>
       </c>
       <c r="CY2" cm="1">
         <f t="array" ref="CY2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CZ2:$HC2,"&gt;0")+1)</f>
-        <v>5.3489936803957595E-3</v>
+        <v>9.8157778538863864E-3</v>
       </c>
       <c r="CZ2" cm="1">
         <f t="array" ref="CZ2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DA2:$HC2,"&gt;0")+1)</f>
-        <v>6.3666769742583788E-3</v>
+        <v>1.1049502719360317E-2</v>
       </c>
       <c r="DA2" cm="1">
         <f t="array" ref="DA2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DB2:$HC2,"&gt;0")+1)</f>
-        <v>7.527256017871682E-3</v>
+        <v>1.2378784364243197E-2</v>
       </c>
       <c r="DB2" cm="1">
         <f t="array" ref="DB2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DC2:$HC2,"&gt;0")+1)</f>
-        <v>8.8401115140645629E-3</v>
+        <v>1.3802533480304061E-2</v>
       </c>
       <c r="DC2" cm="1">
         <f t="array" ref="DC2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DD2:$HC2,"&gt;0")+1)</f>
-        <v>1.0313075211417583E-2</v>
+        <v>1.5318248093427685E-2</v>
       </c>
       <c r="DD2" cm="1">
         <f t="array" ref="DD2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DE2:$HC2,"&gt;0")+1)</f>
-        <v>1.1951953586143727E-2</v>
+        <v>1.6921909457347849E-2</v>
       </c>
       <c r="DE2" cm="1">
         <f t="array" ref="DE2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DF2:$HC2,"&gt;0")+1)</f>
-        <v>1.3760044783996846E-2</v>
+        <v>1.8607902266875063E-2</v>
       </c>
       <c r="DF2" cm="1">
         <f t="array" ref="DF2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DG2:$HC2,"&gt;0")+1)</f>
-        <v>1.573766795613173E-2</v>
+        <v>2.0368963852577183E-2</v>
       </c>
       <c r="DG2" cm="1">
         <f t="array" ref="DG2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DH2:$HC2,"&gt;0")+1)</f>
-        <v>1.7881726451497666E-2</v>
+        <v>2.2196166538662569E-2</v>
       </c>
       <c r="DH2" cm="1">
         <f t="array" ref="DH2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DI2:$HC2,"&gt;0")+1)</f>
-        <v>2.0185327813132176E-2</v>
+        <v>2.4078936668643976E-2</v>
       </c>
       <c r="DI2" cm="1">
         <f t="array" ref="DI2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DJ2:$HC2,"&gt;0")+1)</f>
-        <v>2.2637483954423183E-2</v>
+        <v>2.6005112940459322E-2</v>
       </c>
       <c r="DJ2" cm="1">
         <f t="array" ref="DJ2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DK2:$HC2,"&gt;0")+1)</f>
-        <v>2.5222914095973024E-2</v>
+        <v>2.7961045665188474E-2</v>
       </c>
       <c r="DK2" cm="1">
         <f t="array" ref="DK2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DL2:$HC2,"&gt;0")+1)</f>
-        <v>2.7921970919144796E-2</v>
+        <v>2.993173740221319E-2</v>
       </c>
       <c r="DL2" cm="1">
         <f t="array" ref="DL2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DM2:$HC2,"&gt;0")+1)</f>
-        <v>3.0710706913111802E-2</v>
+        <v>3.1901024168767632E-2</v>
       </c>
       <c r="DM2" cm="1">
         <f t="array" ref="DM2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DN2:$HC2,"&gt;0")+1)</f>
-        <v>3.356109312408851E-2</v>
+        <v>3.3851795121837433E-2</v>
       </c>
       <c r="DN2" cm="1">
         <f t="array" ref="DN2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DO2:$HC2,"&gt;0")+1)</f>
-        <v>3.644139662204475E-2</v>
+        <v>3.576624732108951E-2</v>
       </c>
       <c r="DO2" cm="1">
         <f t="array" ref="DO2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DP2:$HC2,"&gt;0")+1)</f>
-        <v>3.9316716243030805E-2</v>
+        <v>3.7626170965051685E-2</v>
       </c>
       <c r="DP2" cm="1">
         <f t="array" ref="DP2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DQ2:$HC2,"&gt;0")+1)</f>
-        <v>4.2149668897197547E-2</v>
+        <v>3.9413259417212916E-2</v>
       </c>
       <c r="DQ2" cm="1">
         <f t="array" ref="DQ2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DR2:$HC2,"&gt;0")+1)</f>
-        <v>4.4901211387096983E-2</v>
+        <v>4.1109437479695428E-2</v>
       </c>
       <c r="DR2" cm="1">
         <f t="array" ref="DR2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DS2:$HC2,"&gt;0")+1)</f>
-        <v>4.7531575760139111E-2</v>
+        <v>4.2697200818370286E-2</v>
       </c>
       <c r="DS2" cm="1">
         <f t="array" ref="DS2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DT2:$HC2,"&gt;0")+1)</f>
-        <v>5.0001290290909842E-2</v>
+        <v>4.415995931128211E-2</v>
       </c>
       <c r="DT2" cm="1">
         <f t="array" ref="DT2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DU2:$HC2,"&gt;0")+1)</f>
-        <v>5.2272253912054589E-2</v>
+        <v>4.5482377562410338E-2</v>
       </c>
       <c r="DU2" cm="1">
         <f t="array" ref="DU2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DV2:$HC2,"&gt;0")+1)</f>
-        <v>5.4308830141498857E-2</v>
+        <v>4.6650707228810789E-2</v>
       </c>
       <c r="DV2" cm="1">
         <f t="array" ref="DV2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DW2:$HC2,"&gt;0")+1)</f>
-        <v>5.6078928671239994E-2</v>
+        <v>4.7653108874577611E-2</v>
       </c>
       <c r="DW2" cm="1">
         <f t="array" ref="DW2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DX2:$HC2,"&gt;0")+1)</f>
-        <v>5.755505173321445E-2</v>
+        <v>4.8479967596651581E-2</v>
       </c>
       <c r="DX2" cm="1">
         <f t="array" ref="DX2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DY2:$HC2,"&gt;0")+1)</f>
-        <v>5.8715306239949035E-2</v>
+        <v>4.9124221909465797E-2</v>
       </c>
       <c r="DY2" cm="1">
         <f t="array" ref="DY2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DZ2:$HC2,"&gt;0")+1)</f>
-        <v>5.9544449970861169E-2</v>
+        <v>4.9581767885936025E-2</v>
       </c>
       <c r="DZ2" cm="1">
         <f t="array" ref="DZ2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(EA2:$HC2,"&gt;0")+1)</f>
-        <v>6.0035289835080566E-2</v>
+        <v>4.9852160520590598E-2</v>
       </c>
       <c r="EA2" cm="1">
         <f t="array" ref="EA2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(EB2:$HC2,"&gt;0")+1)</f>
-        <v>6.0192694283551618E-2</v>
+        <v>4.9941081907415655E-2</v>
       </c>
       <c r="EB2">
         <v>0</v>
@@ -10711,7 +10728,7 @@
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -10869,7 +10886,7 @@
     </row>
     <row r="2" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B2">
         <f>Calculations!B7</f>
@@ -10877,199 +10894,199 @@
       </c>
       <c r="C2">
         <f>Calculations!C7</f>
-        <v>2.6150091858251345E-3</v>
+        <v>1.7805258402272539E-3</v>
       </c>
       <c r="D2">
         <f>Calculations!D7</f>
-        <v>8.1758556603583749E-3</v>
+        <v>5.4238899945548685E-3</v>
       </c>
       <c r="E2">
         <f>Calculations!E7</f>
-        <v>1.3924786127303026E-2</v>
+        <v>9.2281093631599309E-3</v>
       </c>
       <c r="F2">
         <f>Calculations!F7</f>
-        <v>1.9760682197466944E-2</v>
+        <v>1.3114799334665243E-2</v>
       </c>
       <c r="G2">
         <f>Calculations!G7</f>
-        <v>2.5647150293891575E-2</v>
+        <v>1.7055678109221407E-2</v>
       </c>
       <c r="H2">
         <f>Calculations!H7</f>
-        <v>3.1564414151316167E-2</v>
+        <v>2.1035388234692781E-2</v>
       </c>
       <c r="I2">
         <f>Calculations!I7</f>
-        <v>3.7499909759390417E-2</v>
+        <v>2.5044200523478943E-2</v>
       </c>
       <c r="J2">
         <f>Calculations!J7</f>
-        <v>4.3444914867561142E-2</v>
+        <v>2.9075398473037677E-2</v>
       </c>
       <c r="K2">
         <f>Calculations!K7</f>
-        <v>4.939301598822373E-2</v>
+        <v>3.3124090595303565E-2</v>
       </c>
       <c r="L2">
         <f>Calculations!L7</f>
-        <v>5.533930510353504E-2</v>
+        <v>3.7186590882832007E-2</v>
       </c>
       <c r="M2">
         <f>Calculations!M7</f>
-        <v>6.1279916619134567E-2</v>
+        <v>4.1260064998950227E-2</v>
       </c>
       <c r="N2">
         <f>Calculations!N7</f>
-        <v>6.7211741593422109E-2</v>
+        <v>4.5342315722834106E-2</v>
       </c>
       <c r="O2">
         <f>Calculations!O7</f>
-        <v>7.3132242357491523E-2</v>
+        <v>4.943164813899685E-2</v>
       </c>
       <c r="P2">
         <f>Calculations!P7</f>
-        <v>7.9039327933272382E-2</v>
+        <v>5.3526784123175901E-2</v>
       </c>
       <c r="Q2">
         <f>Calculations!Q7</f>
-        <v>8.4931268491098139E-2</v>
+        <v>5.7626809628520313E-2</v>
       </c>
       <c r="R2">
         <f>Calculations!R7</f>
-        <v>9.0806636325794512E-2</v>
+        <v>6.1731145562481743E-2</v>
       </c>
       <c r="S2">
         <f>Calculations!S7</f>
-        <v>9.6664265964160612E-2</v>
+        <v>6.5839537162283163E-2</v>
       </c>
       <c r="T2">
         <f>Calculations!T7</f>
-        <v>0.10250322907623978</v>
+        <v>6.9952059309580428E-2</v>
       </c>
       <c r="U2">
         <f>Calculations!U7</f>
-        <v>0.10832282183956567</v>
+        <v>7.4069136951086217E-2</v>
       </c>
       <c r="V2">
         <f>Calculations!V7</f>
-        <v>0.11412256382261145</v>
+        <v>7.8191581127134355E-2</v>
       </c>
       <c r="W2">
         <f>Calculations!W7</f>
-        <v>0.11990220861399896</v>
+        <v>8.2320642301122543E-2</v>
       </c>
       <c r="X2">
         <f>Calculations!X7</f>
-        <v>0.12566176752791119</v>
+        <v>8.6458083899014881E-2</v>
       </c>
       <c r="Y2">
         <f>Calculations!Y7</f>
-        <v>0.13140154892198885</v>
+        <v>9.0606280350501611E-2</v>
       </c>
       <c r="Z2">
         <f>Calculations!Z7</f>
-        <v>0.13712221712659151</v>
+        <v>9.4768345615028685E-2</v>
       </c>
       <c r="AA2">
         <f>Calculations!AA7</f>
-        <v>0.14282487688272696</v>
+        <v>9.8948300346039089E-2</v>
       </c>
       <c r="AB2">
         <f>Calculations!AB7</f>
-        <v>0.14851119175410132</v>
+        <v>0.10315128871757681</v>
       </c>
       <c r="AC2">
         <f>Calculations!AC7</f>
-        <v>0.15418354854116612</v>
+        <v>0.10738385981765565</v>
       </c>
       <c r="AD2">
         <f>Calculations!AD7</f>
-        <v>0.1598452847501603</v>
+        <v>0.11165433384728421</v>
       </c>
       <c r="AE2">
         <f>Calculations!AE7</f>
-        <v>0.1655010033487147</v>
+        <v>0.11597328081068911</v>
       </c>
       <c r="AF2">
         <f>Calculations!AF7</f>
-        <v>0.17115700940954851</v>
+        <v>0.12035414993409603</v>
       </c>
       <c r="AG2">
         <f>Calculations!AG7</f>
-        <v>0.17682191839060279</v>
+        <v>0.1248141032382323</v>
       </c>
       <c r="AH2">
         <f>Calculations!AH7</f>
-        <v>0.18250750818851658</v>
+        <v>0.12937512892050151</v>
       </c>
       <c r="AI2">
         <f>Calculations!AI7</f>
-        <v>0.18822992064148872</v>
+        <v>0.13406554334562018</v>
       </c>
       <c r="AJ2">
         <f>Calculations!AJ7</f>
-        <v>0.19401136918487752</v>
+        <v>0.13892204086178234</v>
       </c>
       <c r="AK2">
         <f>Calculations!AK7</f>
-        <v>0.1998825884189582</v>
+        <v>0.14399252908466512</v>
       </c>
       <c r="AL2">
         <f>Calculations!AL7</f>
-        <v>0.2058863864770879</v>
+        <v>0.14934011232493538</v>
       </c>
       <c r="AM2">
         <f>Calculations!AM7</f>
-        <v>0.2120828641903218</v>
+        <v>0.15504879070140029</v>
       </c>
       <c r="AN2">
         <f>Calculations!AN7</f>
-        <v>0.21855720463515754</v>
+        <v>0.16123178854882186</v>
       </c>
       <c r="AO2">
         <f>Calculations!AO7</f>
-        <v>0.22543152441035361</v>
+        <v>0.16804403067447776</v>
       </c>
       <c r="AP2">
         <f>Calculations!AP7</f>
-        <v>0.23288333694124572</v>
+        <v>0.17570138429629648</v>
       </c>
       <c r="AQ2">
         <f>Calculations!AQ7</f>
-        <v>0.24117517665260854</v>
+        <v>0.184511372724845</v>
       </c>
       <c r="AR2">
         <f>Calculations!AR7</f>
-        <v>0.25070391292366057</v>
+        <v>0.19492424341546283</v>
       </c>
       <c r="AS2">
         <f>Calculations!AS7</f>
-        <v>0.26208672199962879</v>
+        <v>0.20762214926878136</v>
       </c>
       <c r="AT2">
         <f>Calculations!AT7</f>
-        <v>0.27631996119753455</v>
+        <v>0.22368449329433546</v>
       </c>
       <c r="AU2">
         <f>Calculations!AU7</f>
-        <v>0.29509538485005954</v>
+        <v>0.244918220042324</v>
       </c>
       <c r="AV2">
         <f>Calculations!AV7</f>
-        <v>0.32149313633984</v>
+        <v>0.27458389943951667</v>
       </c>
       <c r="AW2">
         <f>Calculations!AW7</f>
-        <v>0.36170982122078776</v>
+        <v>0.31921016548691594</v>
       </c>
       <c r="AX2">
         <f>Calculations!AX7</f>
-        <v>0.43023574956437149</v>
+        <v>0.39403596213756642</v>
       </c>
       <c r="AY2">
         <f>Calculations!AY7</f>
-        <v>0.57055284082847824</v>
+        <v>0.54477797773124181</v>
       </c>
       <c r="AZ2">
         <f>Calculations!AZ7</f>

</xml_diff>

<commit_message>
Use heavy-duty rather than light-duty trucks as basis of survival curve for industrial equipment (commit #755e13e; 7/29/24)
</commit_message>
<xml_diff>
--- a/InputData/indst/IESD/Industrial Equipment Survival Data.xlsx
+++ b/InputData/indst/IESD/Industrial Equipment Survival Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\indst\IESD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E332AC6F-E29E-454C-A4B3-7772407E5D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{64B90A02-37DE-4644-92CE-A9ED6E1F2E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61980" yWindow="3210" windowWidth="21600" windowHeight="12525" xr2:uid="{F6F8D70B-4981-4594-95C7-E07791D5C609}"/>
+    <workbookView xWindow="61980" yWindow="3210" windowWidth="21600" windowHeight="12525" activeTab="1" xr2:uid="{F6F8D70B-4981-4594-95C7-E07791D5C609}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -140,18 +140,12 @@
     <t>To estimate a survival curve for heterogenous mixes of industrial equipment in each ISIC code,</t>
   </si>
   <si>
-    <t>we use a Weibull function to curve fit survival curve data for light commerical trucks from the</t>
-  </si>
-  <si>
     <t>MOVE3 model.  We extend our curve fit to 50 years to avoid a discontinuity in the MOVES3 data</t>
   </si>
   <si>
     <t>where they retire an unusually large share of the remaining stock in year 30.</t>
   </si>
   <si>
-    <t xml:space="preserve">After 50 years, the share of surviving equipment from the curve fit would be just 0.035%.  </t>
-  </si>
-  <si>
     <t>so that we can capture the full lifetime of all industrial equipment and avoid problems with a</t>
   </si>
   <si>
@@ -837,16 +831,23 @@
   </si>
   <si>
     <t>We set this to zero and smoothly adjust the remainder of the Weibull curve accordingly,</t>
+  </si>
+  <si>
+    <t>we use a Weibull function to curve fit survival curve data for heavy-duty commerical trucks from the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After 50 years, the share of surviving equipment from the curve fit would be just 0.5%.  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -883,6 +884,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -1005,10 +1013,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1054,12 +1063,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1154,154 +1165,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>6.0192694283551618E-2</c:v>
+                  <c:v>4.9941081907415655E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0035289835080566E-2</c:v>
+                  <c:v>4.9852160520590598E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9544449970861169E-2</c:v>
+                  <c:v>4.9581767885936025E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8715306239949035E-2</c:v>
+                  <c:v>4.9124221909465797E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.755505173321445E-2</c:v>
+                  <c:v>4.8479967596651581E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.6078928671239994E-2</c:v>
+                  <c:v>4.7653108874577611E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.4308830141498857E-2</c:v>
+                  <c:v>4.6650707228810789E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.2272253912054589E-2</c:v>
+                  <c:v>4.5482377562410338E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0001290290909842E-2</c:v>
+                  <c:v>4.415995931128211E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.7531575760139111E-2</c:v>
+                  <c:v>4.2697200818370286E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.4901211387096983E-2</c:v>
+                  <c:v>4.1109437479695428E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.2149668897197547E-2</c:v>
+                  <c:v>3.9413259417212916E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.9316716243030805E-2</c:v>
+                  <c:v>3.7626170965051685E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.644139662204475E-2</c:v>
+                  <c:v>3.576624732108951E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.356109312408851E-2</c:v>
+                  <c:v>3.3851795121837433E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.0710706913111802E-2</c:v>
+                  <c:v>3.1901024168767632E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.7921970919144796E-2</c:v>
+                  <c:v>2.993173740221319E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.5222914095973024E-2</c:v>
+                  <c:v>2.7961045665188474E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.2637483954423183E-2</c:v>
+                  <c:v>2.6005112940459322E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0185327813132176E-2</c:v>
+                  <c:v>2.4078936668643976E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.7881726451497666E-2</c:v>
+                  <c:v>2.2196166538662569E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.573766795613173E-2</c:v>
+                  <c:v>2.0368963852577183E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.3760044783996846E-2</c:v>
+                  <c:v>1.8607902266875063E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.1951953586143727E-2</c:v>
+                  <c:v>1.6921909457347849E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.0313075211417583E-2</c:v>
+                  <c:v>1.5318248093427685E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.8401115140645629E-3</c:v>
+                  <c:v>1.3802533480304061E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.527256017871682E-3</c:v>
+                  <c:v>1.2378784364243197E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.3666769742583788E-3</c:v>
+                  <c:v>1.1049502719360317E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.3489936803957595E-3</c:v>
+                  <c:v>9.8157778538863864E-3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.4637298593843263E-3</c:v>
+                  <c:v>8.6774098924622765E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.6997312058400008E-3</c:v>
+                  <c:v>7.6330476012252636E-3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0455376364937939E-3</c:v>
+                  <c:v>6.680335609903592E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.4897041513629674E-3</c:v>
+                  <c:v>5.8160663291400979E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.0210673365311312E-3</c:v>
+                  <c:v>5.0363322365897644E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.6289572953558926E-3</c:v>
+                  <c:v>4.336674683824729E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.3033570947362115E-3</c:v>
+                  <c:v>3.712225928283366E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.0350136122116973E-3</c:v>
+                  <c:v>3.1578416911779905E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.155049608578695E-4</c:v>
+                  <c:v>2.6682221557343786E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6.3727047624667003E-4</c:v>
+                  <c:v>2.2380199253197314E-3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.9360962132467118E-4</c:v>
+                  <c:v>1.8619340363392101E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.7865616556427702E-4</c:v>
+                  <c:v>1.53478964868602E-3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.8733369794371315E-4</c:v>
+                  <c:v>1.2516035037630799E-3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.1529801555439907E-4</c:v>
+                  <c:v>1.0076356377359192E-3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.5887126440472155E-4</c:v>
+                  <c:v>7.9842816094936842E-4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.1497196278900563E-4</c:v>
+                  <c:v>6.1983216233548084E-4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>8.1044267182817299E-5</c:v>
+                  <c:v>4.6802397241129008E-4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5.4989091543849397E-5</c:v>
+                  <c:v>3.395121250354253E-4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.5098997072430095E-5</c:v>
+                  <c:v>2.3113640341805268E-4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.9998153758015452E-5</c:v>
+                  <c:v>1.4006034831220358E-4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>8.5881503200550279E-6</c:v>
+                  <c:v>6.3758554998347974E-5</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>0</c:v>
@@ -1764,94 +1775,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.99099999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99099999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99099999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98599999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98099999999999998</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.97599999999999998</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.97</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.96399999999999997</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.95799999999999996</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.95199999999999996</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.94599999999999995</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>0.94</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.93500000000000005</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.92900000000000005</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.91300000000000003</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.90800000000000003</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.90300000000000002</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.89800000000000002</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.89400000000000002</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.89100000000000001</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.88800000000000001</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.88500000000000001</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.88300000000000001</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.88</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.879</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.877</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.875</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.875</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.873</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.872</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0.3</c:v>
@@ -2076,94 +2087,94 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99099999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98208099999999998</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96833186599999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.94993356054599998</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.92713515509289601</c:v>
+                  <c:v>0.97019999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.89932110044010916</c:v>
+                  <c:v>0.95079599999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.86694554082426523</c:v>
+                  <c:v>0.92227211999999992</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.83053382810964604</c:v>
+                  <c:v>0.8946039563999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.79066820436038299</c:v>
+                  <c:v>0.86776583770799987</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.7479721213249223</c:v>
+                  <c:v>0.83305520419967982</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.70309379404542693</c:v>
+                  <c:v>0.79973299603169257</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.65739269743247419</c:v>
+                  <c:v>0.75974634623010795</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.61071781591476859</c:v>
+                  <c:v>0.72175902891860255</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.55758536593018371</c:v>
+                  <c:v>0.68567107747267242</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.50628751226460678</c:v>
+                  <c:v>0.64453081282431202</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.45717762357493991</c:v>
+                  <c:v>0.60585896405485329</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.41054550597029604</c:v>
+                  <c:v>0.56344883657101363</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.36702768233744465</c:v>
+                  <c:v>0.52400741801104267</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.32702166496266316</c:v>
+                  <c:v>0.48208682457015928</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.2903952384868449</c:v>
+                  <c:v>0.44351987860454656</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.25699978606085772</c:v>
+                  <c:v>0.40803828831618283</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.22693081109173738</c:v>
+                  <c:v>0.37131484236772638</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.19969911376072888</c:v>
+                  <c:v>0.33789650655463099</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.17553552099568068</c:v>
+                  <c:v>0.30748582096471422</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.15394465191321197</c:v>
+                  <c:v>0.27673723886824281</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.13470157042406047</c:v>
+                  <c:v>0.24906351498141854</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.11786387412105291</c:v>
+                  <c:v>0.22415716348327669</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.1028951621076792</c:v>
+                  <c:v>0.19949987550011625</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8.9724581357896266E-2</c:v>
+                  <c:v>0.17755488919510345</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.6917374407368879E-2</c:v>
+                  <c:v>5.3266466758531035E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2202,9 +2213,7 @@
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent3"/>
@@ -2385,154 +2394,154 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99739212515354392</c:v>
+                  <c:v>0.99831675588711721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98924478377020841</c:v>
+                  <c:v>0.99299980499619667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.97547709475632682</c:v>
+                  <c:v>0.98393537137827769</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.95620855917354664</c:v>
+                  <c:v>0.97113236564271588</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9316924007853824</c:v>
+                  <c:v>0.95467296316352146</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9022923362809403</c:v>
+                  <c:v>0.93469856026807085</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.86846519465567973</c:v>
+                  <c:v>0.911401681881576</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.83074410220315842</c:v>
+                  <c:v>0.88501939607412372</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.78972109891259246</c:v>
+                  <c:v>0.85582699409730667</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.74602916969698607</c:v>
+                  <c:v>0.82413154571082692</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.7003240706390983</c:v>
+                  <c:v>0.79026524479839177</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.653266479136134</c:v>
+                  <c:v>0.75457859105805325</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.60550503200212358</c:v>
+                  <c:v>0.71743351493239338</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.55766078616588688</c:v>
+                  <c:v>0.67919658109746339</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.51031356554733853</c:v>
+                  <c:v>0.64023241524371066</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.46399055920833854</c:v>
+                  <c:v>0.60089749623889543</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.41915742089838504</c:v>
+                  <c:v>0.56153444467433955</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.37621199808238615</c:v>
+                  <c:v>0.52246692159518826</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.33548069779147327</c:v>
+                  <c:v>0.48399522967902553</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.2972173843787802</c:v>
+                  <c:v>0.44639268476921745</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.26160460635360461</c:v>
+                  <c:v>0.4099027998534206</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.22875687025273661</c:v>
+                  <c:v>0.37473729754723328</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.1987256217057094</c:v>
+                  <c:v>0.34107494201536037</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.1715055585548676</c:v>
+                  <c:v>0.30906115800942446</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.14704188767634285</c:v>
+                  <c:v>0.27880838412656883</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.12523814427017732</c:v>
+                  <c:v>0.25039709011459887</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.10596421705503067</c:v>
+                  <c:v>0.22387737448999978</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8.9064261489625096E-2</c:v>
+                  <c:v>0.19927104911966265</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.4364231919015422E-2</c:v>
+                  <c:v>0.17657411178033777</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6.1678818389612644E-2</c:v>
+                  <c:v>0.15575950591235288</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.0817630964475224E-2</c:v>
+                  <c:v>0.13678006853521585</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.1590530289999483E-2</c:v>
+                  <c:v>0.1195715721785825</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.3812055089708859E-2</c:v>
+                  <c:v>0.10405577419740442</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.7304943043493068E-2</c:v>
+                  <c:v>9.0143396421134003E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.1902779718167675E-2</c:v>
+                  <c:v>7.773696914395567E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.7451840104900196E-2</c:v>
+                  <c:v>6.6733485410649274E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.3812208770020096E-2</c:v>
+                  <c:v>5.7026823836338725E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.085827803774464E-2</c:v>
+                  <c:v>4.8509910316327787E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.4787297965790431E-3</c:v>
+                  <c:v>4.1076600502268801E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.5761065295036891E-3</c:v>
+                  <c:v>3.4623275491463823E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.0660722372383171E-3</c:v>
+                  <c:v>2.9050152531782669E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.8764553222113696E-3</c:v>
+                  <c:v>2.4262320506897139E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.9461544491962144E-3</c:v>
+                  <c:v>2.0170516439616759E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.2239760017190857E-3</c:v>
+                  <c:v>1.6691664214857793E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.6674589543207441E-3</c:v>
+                  <c:v>1.3749200223324487E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.2417305360230557E-3</c:v>
+                  <c:v>1.1273212760904316E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>9.1842453361701271E-4</c:v>
+                  <c:v>9.2004229263573656E-3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6.7468385411284526E-4</c:v>
+                  <c:v>7.47403460837337E-3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.9226024838955329E-4</c:v>
+                  <c:v>6.0434801255350168E-3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.5671696845152034E-4</c:v>
+                  <c:v>4.8640863672232415E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2842,151 +2851,151 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6150091858251345E-3</c:v>
+                  <c:v>1.7805258402272539E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.1758556603583749E-3</c:v>
+                  <c:v>5.4238899945548685E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3924786127303026E-2</c:v>
+                  <c:v>9.2281093631599309E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9760682197466944E-2</c:v>
+                  <c:v>1.3114799334665243E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5647150293891575E-2</c:v>
+                  <c:v>1.7055678109221407E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1564414151316167E-2</c:v>
+                  <c:v>2.1035388234692781E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7499909759390417E-2</c:v>
+                  <c:v>2.5044200523478943E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.3444914867561142E-2</c:v>
+                  <c:v>2.9075398473037677E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.939301598822373E-2</c:v>
+                  <c:v>3.3124090595303565E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.533930510353504E-2</c:v>
+                  <c:v>3.7186590882832007E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.1279916619134567E-2</c:v>
+                  <c:v>4.1260064998950227E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.7211741593422109E-2</c:v>
+                  <c:v>4.5342315722834106E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.3132242357491523E-2</c:v>
+                  <c:v>4.943164813899685E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.9039327933272382E-2</c:v>
+                  <c:v>5.3526784123175901E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.4931268491098139E-2</c:v>
+                  <c:v>5.7626809628520313E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.0806636325794512E-2</c:v>
+                  <c:v>6.1731145562481743E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.6664265964160612E-2</c:v>
+                  <c:v>6.5839537162283163E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.10250322907623978</c:v>
+                  <c:v>6.9952059309580428E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.10832282183956567</c:v>
+                  <c:v>7.4069136951086217E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.11412256382261145</c:v>
+                  <c:v>7.8191581127134355E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.11990220861399896</c:v>
+                  <c:v>8.2320642301122543E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.12566176752791119</c:v>
+                  <c:v>8.6458083899014881E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.13140154892198885</c:v>
+                  <c:v>9.0606280350501611E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.13712221712659151</c:v>
+                  <c:v>9.4768345615028685E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.14282487688272696</c:v>
+                  <c:v>9.8948300346039089E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.14851119175410132</c:v>
+                  <c:v>0.10315128871757681</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.15418354854116612</c:v>
+                  <c:v>0.10738385981765565</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.1598452847501603</c:v>
+                  <c:v>0.11165433384728421</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.1655010033487147</c:v>
+                  <c:v>0.11597328081068911</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.17115700940954851</c:v>
+                  <c:v>0.12035414993409603</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.17682191839060279</c:v>
+                  <c:v>0.1248141032382323</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.18250750818851658</c:v>
+                  <c:v>0.12937512892050151</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.18822992064148872</c:v>
+                  <c:v>0.13406554334562018</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.19401136918487752</c:v>
+                  <c:v>0.13892204086178234</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.1998825884189582</c:v>
+                  <c:v>0.14399252908466512</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.2058863864770879</c:v>
+                  <c:v>0.14934011232493538</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.2120828641903218</c:v>
+                  <c:v>0.15504879070140029</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.21855720463515754</c:v>
+                  <c:v>0.16123178854882186</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.22543152441035361</c:v>
+                  <c:v>0.16804403067447776</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.23288333694124572</c:v>
+                  <c:v>0.17570138429629648</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.24117517665260854</c:v>
+                  <c:v>0.184511372724845</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.25070391292366057</c:v>
+                  <c:v>0.19492424341546283</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.26208672199962879</c:v>
+                  <c:v>0.20762214926878136</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.27631996119753455</c:v>
+                  <c:v>0.22368449329433546</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.29509538485005954</c:v>
+                  <c:v>0.244918220042324</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.32149313633984</c:v>
+                  <c:v>0.27458389943951667</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.36170982122078776</c:v>
+                  <c:v>0.31921016548691594</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.43023574956437149</c:v>
+                  <c:v>0.39403596213756642</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.57055284082847824</c:v>
+                  <c:v>0.54477797773124181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4125,154 +4134,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>8.5881503200550279E-6</c:v>
+                  <c:v>6.3758554998347974E-5</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.9998153758015452E-5</c:v>
+                  <c:v>1.4006034831220358E-4</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>3.5098997072430095E-5</c:v>
+                  <c:v>2.3113640341805268E-4</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>5.4989091543849397E-5</c:v>
+                  <c:v>3.395121250354253E-4</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>8.1044267182817299E-5</c:v>
+                  <c:v>4.6802397241129008E-4</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.1497196278900563E-4</c:v>
+                  <c:v>6.1983216233548084E-4</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.5887126440472155E-4</c:v>
+                  <c:v>7.9842816094936842E-4</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2.1529801555439907E-4</c:v>
+                  <c:v>1.0076356377359192E-3</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2.8733369794371315E-4</c:v>
+                  <c:v>1.2516035037630799E-3</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>3.7865616556427702E-4</c:v>
+                  <c:v>1.53478964868602E-3</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>4.9360962132467118E-4</c:v>
+                  <c:v>1.8619340363392101E-3</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>6.3727047624667003E-4</c:v>
+                  <c:v>2.2380199253197314E-3</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>8.155049608578695E-4</c:v>
+                  <c:v>2.6682221557343786E-3</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1.0350136122116973E-3</c:v>
+                  <c:v>3.1578416911779905E-3</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.3033570947362115E-3</c:v>
+                  <c:v>3.712225928283366E-3</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.6289572953558926E-3</c:v>
+                  <c:v>4.336674683824729E-3</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2.0210673365311312E-3</c:v>
+                  <c:v>5.0363322365897644E-3</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2.4897041513629674E-3</c:v>
+                  <c:v>5.8160663291400979E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>3.0455376364937939E-3</c:v>
+                  <c:v>6.680335609903592E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>3.6997312058400008E-3</c:v>
+                  <c:v>7.6330476012252636E-3</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>4.4637298593843263E-3</c:v>
+                  <c:v>8.6774098924622765E-3</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>5.3489936803957595E-3</c:v>
+                  <c:v>9.8157778538863864E-3</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>6.3666769742583788E-3</c:v>
+                  <c:v>1.1049502719360317E-2</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>7.527256017871682E-3</c:v>
+                  <c:v>1.2378784364243197E-2</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>8.8401115140645629E-3</c:v>
+                  <c:v>1.3802533480304061E-2</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1.0313075211417583E-2</c:v>
+                  <c:v>1.5318248093427685E-2</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1.1951953586143727E-2</c:v>
+                  <c:v>1.6921909457347849E-2</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1.3760044783996846E-2</c:v>
+                  <c:v>1.8607902266875063E-2</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1.573766795613173E-2</c:v>
+                  <c:v>2.0368963852577183E-2</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1.7881726451497666E-2</c:v>
+                  <c:v>2.2196166538662569E-2</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>2.0185327813132176E-2</c:v>
+                  <c:v>2.4078936668643976E-2</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>2.2637483954423183E-2</c:v>
+                  <c:v>2.6005112940459322E-2</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>2.5222914095973024E-2</c:v>
+                  <c:v>2.7961045665188474E-2</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>2.7921970919144796E-2</c:v>
+                  <c:v>2.993173740221319E-2</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>3.0710706913111802E-2</c:v>
+                  <c:v>3.1901024168767632E-2</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>3.356109312408851E-2</c:v>
+                  <c:v>3.3851795121837433E-2</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>3.644139662204475E-2</c:v>
+                  <c:v>3.576624732108951E-2</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>3.9316716243030805E-2</c:v>
+                  <c:v>3.7626170965051685E-2</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>4.2149668897197547E-2</c:v>
+                  <c:v>3.9413259417212916E-2</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>4.4901211387096983E-2</c:v>
+                  <c:v>4.1109437479695428E-2</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>4.7531575760139111E-2</c:v>
+                  <c:v>4.2697200818370286E-2</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>5.0001290290909842E-2</c:v>
+                  <c:v>4.415995931128211E-2</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>5.2272253912054589E-2</c:v>
+                  <c:v>4.5482377562410338E-2</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>5.4308830141498857E-2</c:v>
+                  <c:v>4.6650707228810789E-2</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>5.6078928671239994E-2</c:v>
+                  <c:v>4.7653108874577611E-2</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>5.755505173321445E-2</c:v>
+                  <c:v>4.8479967596651581E-2</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>5.8715306239949035E-2</c:v>
+                  <c:v>4.9124221909465797E-2</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>5.9544449970861169E-2</c:v>
+                  <c:v>4.9581767885936025E-2</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>6.0035289835080566E-2</c:v>
+                  <c:v>4.9852160520590598E-2</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>6.0192694283551618E-2</c:v>
+                  <c:v>4.9941081907415655E-2</c:v>
                 </c:pt>
                 <c:pt idx="130">
                   <c:v>0</c:v>
@@ -7390,9 +7399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277D797A-29C7-42A2-8124-270B3E72FA7C}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -7401,12 +7408,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -7449,57 +7456,57 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B24" s="12"/>
     </row>
@@ -7512,17 +7519,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B12B9A-7BC4-4CDD-8298-A2C7A60D90EB}">
   <dimension ref="A1:AZ12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="53.453125" customWidth="1"/>
     <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -7683,95 +7691,95 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <f t="array" ref="B2:AF2">TRANSPOSE('MOVES3 Table C-1'!D3:D33)</f>
-        <v>0.99099999999999999</v>
+        <f t="array" ref="B2:AF2">TRANSPOSE('MOVES3 Table C-1'!E3:E33)</f>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0.99099999999999999</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0.99099999999999999</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.98599999999999999</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0.98099999999999998</v>
+        <v>0.99</v>
       </c>
       <c r="G2">
-        <v>0.97599999999999998</v>
+        <v>0.98</v>
       </c>
       <c r="H2">
+        <v>0.98</v>
+      </c>
+      <c r="I2">
         <v>0.97</v>
       </c>
-      <c r="I2">
-        <v>0.96399999999999997</v>
-      </c>
       <c r="J2">
-        <v>0.95799999999999996</v>
+        <v>0.97</v>
       </c>
       <c r="K2">
-        <v>0.95199999999999996</v>
+        <v>0.97</v>
       </c>
       <c r="L2">
-        <v>0.94599999999999995</v>
+        <v>0.96</v>
       </c>
       <c r="M2">
+        <v>0.96</v>
+      </c>
+      <c r="N2">
+        <v>0.95</v>
+      </c>
+      <c r="O2">
+        <v>0.95</v>
+      </c>
+      <c r="P2">
+        <v>0.95</v>
+      </c>
+      <c r="Q2">
         <v>0.94</v>
       </c>
-      <c r="N2">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="O2">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="P2">
-        <v>0.91300000000000003</v>
-      </c>
-      <c r="Q2">
-        <v>0.90800000000000003</v>
-      </c>
       <c r="R2">
-        <v>0.90300000000000002</v>
+        <v>0.94</v>
       </c>
       <c r="S2">
-        <v>0.89800000000000002</v>
+        <v>0.93</v>
       </c>
       <c r="T2">
-        <v>0.89400000000000002</v>
+        <v>0.93</v>
       </c>
       <c r="U2">
-        <v>0.89100000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="V2">
-        <v>0.88800000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="W2">
-        <v>0.88500000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="X2">
-        <v>0.88300000000000001</v>
+        <v>0.91</v>
       </c>
       <c r="Y2">
-        <v>0.88</v>
+        <v>0.91</v>
       </c>
       <c r="Z2">
-        <v>0.879</v>
+        <v>0.91</v>
       </c>
       <c r="AA2">
-        <v>0.877</v>
+        <v>0.9</v>
       </c>
       <c r="AB2">
-        <v>0.875</v>
+        <v>0.9</v>
       </c>
       <c r="AC2">
-        <v>0.875</v>
+        <v>0.9</v>
       </c>
       <c r="AD2">
-        <v>0.873</v>
+        <v>0.89</v>
       </c>
       <c r="AE2">
-        <v>0.872</v>
+        <v>0.89</v>
       </c>
       <c r="AF2">
         <v>0.3</v>
@@ -7786,123 +7794,123 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:AF3" si="0">B3*C2</f>
-        <v>0.99099999999999999</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
-        <v>0.98208099999999998</v>
+        <f>C3*D2</f>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>0.96833186599999999</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>0.94993356054599998</v>
+        <v>0.99</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>0.92713515509289601</v>
+        <v>0.97019999999999995</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>0.89932110044010916</v>
+        <v>0.95079599999999997</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
-        <v>0.86694554082426523</v>
+        <v>0.92227211999999992</v>
       </c>
       <c r="J3">
         <f t="shared" si="0"/>
-        <v>0.83053382810964604</v>
+        <v>0.8946039563999999</v>
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
-        <v>0.79066820436038299</v>
+        <v>0.86776583770799987</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>0.7479721213249223</v>
+        <v>0.83305520419967982</v>
       </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>0.70309379404542693</v>
+        <v>0.79973299603169257</v>
       </c>
       <c r="N3">
         <f t="shared" si="0"/>
-        <v>0.65739269743247419</v>
+        <v>0.75974634623010795</v>
       </c>
       <c r="O3">
         <f t="shared" si="0"/>
-        <v>0.61071781591476859</v>
+        <v>0.72175902891860255</v>
       </c>
       <c r="P3">
         <f t="shared" si="0"/>
-        <v>0.55758536593018371</v>
+        <v>0.68567107747267242</v>
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
-        <v>0.50628751226460678</v>
+        <v>0.64453081282431202</v>
       </c>
       <c r="R3">
         <f t="shared" si="0"/>
-        <v>0.45717762357493991</v>
+        <v>0.60585896405485329</v>
       </c>
       <c r="S3">
         <f t="shared" si="0"/>
-        <v>0.41054550597029604</v>
+        <v>0.56344883657101363</v>
       </c>
       <c r="T3">
         <f t="shared" si="0"/>
-        <v>0.36702768233744465</v>
+        <v>0.52400741801104267</v>
       </c>
       <c r="U3">
         <f t="shared" si="0"/>
-        <v>0.32702166496266316</v>
+        <v>0.48208682457015928</v>
       </c>
       <c r="V3">
         <f t="shared" si="0"/>
-        <v>0.2903952384868449</v>
+        <v>0.44351987860454656</v>
       </c>
       <c r="W3">
         <f t="shared" si="0"/>
-        <v>0.25699978606085772</v>
+        <v>0.40803828831618283</v>
       </c>
       <c r="X3">
         <f t="shared" si="0"/>
-        <v>0.22693081109173738</v>
+        <v>0.37131484236772638</v>
       </c>
       <c r="Y3">
         <f t="shared" si="0"/>
-        <v>0.19969911376072888</v>
+        <v>0.33789650655463099</v>
       </c>
       <c r="Z3">
         <f t="shared" si="0"/>
-        <v>0.17553552099568068</v>
+        <v>0.30748582096471422</v>
       </c>
       <c r="AA3">
         <f t="shared" si="0"/>
-        <v>0.15394465191321197</v>
+        <v>0.27673723886824281</v>
       </c>
       <c r="AB3">
         <f t="shared" si="0"/>
-        <v>0.13470157042406047</v>
+        <v>0.24906351498141854</v>
       </c>
       <c r="AC3">
         <f t="shared" si="0"/>
-        <v>0.11786387412105291</v>
+        <v>0.22415716348327669</v>
       </c>
       <c r="AD3">
         <f t="shared" si="0"/>
-        <v>0.1028951621076792</v>
+        <v>0.19949987550011625</v>
       </c>
       <c r="AE3">
         <f t="shared" si="0"/>
-        <v>8.9724581357896266E-2</v>
+        <v>0.17755488919510345</v>
       </c>
       <c r="AF3">
         <f t="shared" si="0"/>
-        <v>2.6917374407368879E-2</v>
+        <v>5.3266466758531035E-2</v>
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.35">
@@ -7915,203 +7923,203 @@
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>0.99739212515354392</v>
+        <v>0.99831675588711721</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>0.98924478377020841</v>
+        <v>0.99299980499619667</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>0.97547709475632682</v>
+        <v>0.98393537137827769</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>0.95620855917354664</v>
+        <v>0.97113236564271588</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>0.9316924007853824</v>
+        <v>0.95467296316352146</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
-        <v>0.9022923362809403</v>
+        <v>0.93469856026807085</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>0.86846519465567973</v>
+        <v>0.911401681881576</v>
       </c>
       <c r="J4">
         <f t="shared" si="1"/>
-        <v>0.83074410220315842</v>
+        <v>0.88501939607412372</v>
       </c>
       <c r="K4">
         <f t="shared" si="1"/>
-        <v>0.78972109891259246</v>
+        <v>0.85582699409730667</v>
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>0.74602916969698607</v>
+        <v>0.82413154571082692</v>
       </c>
       <c r="M4">
         <f t="shared" si="1"/>
-        <v>0.7003240706390983</v>
+        <v>0.79026524479839177</v>
       </c>
       <c r="N4">
         <f t="shared" si="1"/>
-        <v>0.653266479136134</v>
+        <v>0.75457859105805325</v>
       </c>
       <c r="O4">
         <f t="shared" si="1"/>
-        <v>0.60550503200212358</v>
+        <v>0.71743351493239338</v>
       </c>
       <c r="P4">
         <f t="shared" si="1"/>
-        <v>0.55766078616588688</v>
+        <v>0.67919658109746339</v>
       </c>
       <c r="Q4">
         <f t="shared" si="1"/>
-        <v>0.51031356554733853</v>
+        <v>0.64023241524371066</v>
       </c>
       <c r="R4">
         <f t="shared" si="1"/>
-        <v>0.46399055920833854</v>
+        <v>0.60089749623889543</v>
       </c>
       <c r="S4">
         <f t="shared" si="1"/>
-        <v>0.41915742089838504</v>
+        <v>0.56153444467433955</v>
       </c>
       <c r="T4">
         <f t="shared" si="1"/>
-        <v>0.37621199808238615</v>
+        <v>0.52246692159518826</v>
       </c>
       <c r="U4">
         <f t="shared" si="1"/>
-        <v>0.33548069779147327</v>
+        <v>0.48399522967902553</v>
       </c>
       <c r="V4">
         <f t="shared" si="1"/>
-        <v>0.2972173843787802</v>
+        <v>0.44639268476921745</v>
       </c>
       <c r="W4">
         <f t="shared" si="1"/>
-        <v>0.26160460635360461</v>
+        <v>0.4099027998534206</v>
       </c>
       <c r="X4">
         <f t="shared" si="1"/>
-        <v>0.22875687025273661</v>
+        <v>0.37473729754723328</v>
       </c>
       <c r="Y4">
         <f t="shared" si="1"/>
-        <v>0.1987256217057094</v>
+        <v>0.34107494201536037</v>
       </c>
       <c r="Z4">
         <f t="shared" si="1"/>
-        <v>0.1715055585548676</v>
+        <v>0.30906115800942446</v>
       </c>
       <c r="AA4">
         <f t="shared" si="1"/>
-        <v>0.14704188767634285</v>
+        <v>0.27880838412656883</v>
       </c>
       <c r="AB4">
         <f t="shared" si="1"/>
-        <v>0.12523814427017732</v>
+        <v>0.25039709011459887</v>
       </c>
       <c r="AC4">
         <f t="shared" si="1"/>
-        <v>0.10596421705503067</v>
+        <v>0.22387737448999978</v>
       </c>
       <c r="AD4">
         <f t="shared" si="1"/>
-        <v>8.9064261489625096E-2</v>
+        <v>0.19927104911966265</v>
       </c>
       <c r="AE4">
         <f t="shared" si="1"/>
-        <v>7.4364231919015422E-2</v>
+        <v>0.17657411178033777</v>
       </c>
       <c r="AF4">
         <f t="shared" si="1"/>
-        <v>6.1678818389612644E-2</v>
+        <v>0.15575950591235288</v>
       </c>
       <c r="AG4">
         <f t="shared" ref="AG4:AZ4" si="2">1-_xlfn.WEIBULL.DIST(AG1,$B$10,$B$12,TRUE)</f>
-        <v>5.0817630964475224E-2</v>
+        <v>0.13678006853521585</v>
       </c>
       <c r="AH4">
         <f t="shared" si="2"/>
-        <v>4.1590530289999483E-2</v>
+        <v>0.1195715721785825</v>
       </c>
       <c r="AI4">
         <f t="shared" si="2"/>
-        <v>3.3812055089708859E-2</v>
+        <v>0.10405577419740442</v>
       </c>
       <c r="AJ4">
         <f t="shared" si="2"/>
-        <v>2.7304943043493068E-2</v>
+        <v>9.0143396421134003E-2</v>
       </c>
       <c r="AK4">
         <f t="shared" si="2"/>
-        <v>2.1902779718167675E-2</v>
+        <v>7.773696914395567E-2</v>
       </c>
       <c r="AL4">
         <f t="shared" si="2"/>
-        <v>1.7451840104900196E-2</v>
+        <v>6.6733485410649274E-2</v>
       </c>
       <c r="AM4">
         <f t="shared" si="2"/>
-        <v>1.3812208770020096E-2</v>
+        <v>5.7026823836338725E-2</v>
       </c>
       <c r="AN4">
         <f t="shared" si="2"/>
-        <v>1.085827803774464E-2</v>
+        <v>4.8509910316327787E-2</v>
       </c>
       <c r="AO4">
         <f t="shared" si="2"/>
-        <v>8.4787297965790431E-3</v>
+        <v>4.1076600502268801E-2</v>
       </c>
       <c r="AP4">
         <f t="shared" si="2"/>
-        <v>6.5761065295036891E-3</v>
+        <v>3.4623275491463823E-2</v>
       </c>
       <c r="AQ4">
         <f t="shared" si="2"/>
-        <v>5.0660722372383171E-3</v>
+        <v>2.9050152531782669E-2</v>
       </c>
       <c r="AR4">
         <f t="shared" si="2"/>
-        <v>3.8764553222113696E-3</v>
+        <v>2.4262320506897139E-2</v>
       </c>
       <c r="AS4">
         <f t="shared" si="2"/>
-        <v>2.9461544491962144E-3</v>
+        <v>2.0170516439616759E-2</v>
       </c>
       <c r="AT4">
         <f t="shared" si="2"/>
-        <v>2.2239760017190857E-3</v>
+        <v>1.6691664214857793E-2</v>
       </c>
       <c r="AU4">
         <f t="shared" si="2"/>
-        <v>1.6674589543207441E-3</v>
+        <v>1.3749200223324487E-2</v>
       </c>
       <c r="AV4">
         <f t="shared" si="2"/>
-        <v>1.2417305360230557E-3</v>
+        <v>1.1273212760904316E-2</v>
       </c>
       <c r="AW4">
         <f t="shared" si="2"/>
-        <v>9.1842453361701271E-4</v>
+        <v>9.2004229263573656E-3</v>
       </c>
       <c r="AX4">
         <f t="shared" si="2"/>
-        <v>6.7468385411284526E-4</v>
+        <v>7.47403460837337E-3</v>
       </c>
       <c r="AY4">
         <f t="shared" si="2"/>
-        <v>4.9226024838955329E-4</v>
+        <v>6.0434801255350168E-3</v>
       </c>
       <c r="AZ4">
         <f t="shared" si="2"/>
-        <v>3.5671696845152034E-4</v>
+        <v>4.8640863672232415E-3</v>
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.35">
@@ -8124,199 +8132,199 @@
       </c>
       <c r="C5">
         <f t="shared" ref="C5" si="4">C4-(C1/$AZ$1)*$AZ$4</f>
-        <v>0.99738499081417487</v>
+        <v>0.99821947415977275</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5" si="5">D4-(D1/$AZ$1)*$AZ$4</f>
-        <v>0.98923051509147031</v>
+        <v>0.99280524154150773</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5" si="6">E4-(E1/$AZ$1)*$AZ$4</f>
-        <v>0.97545569173821978</v>
+        <v>0.98364352619624429</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5" si="7">F4-(F1/$AZ$1)*$AZ$4</f>
-        <v>0.95618002181607054</v>
+        <v>0.97074323873333801</v>
       </c>
       <c r="G5">
         <f t="shared" ref="G5" si="8">G4-(G1/$AZ$1)*$AZ$4</f>
-        <v>0.93165672908853725</v>
+        <v>0.95418655452679912</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5" si="9">H4-(H1/$AZ$1)*$AZ$4</f>
-        <v>0.90224953024472609</v>
+        <v>0.93411486990400405</v>
       </c>
       <c r="I5">
         <f t="shared" ref="I5" si="10">I4-(I1/$AZ$1)*$AZ$4</f>
-        <v>0.86841525428009647</v>
+        <v>0.91072070979016473</v>
       </c>
       <c r="J5">
         <f t="shared" ref="J5" si="11">J4-(J1/$AZ$1)*$AZ$4</f>
-        <v>0.83068702748820622</v>
+        <v>0.88424114225536798</v>
       </c>
       <c r="K5">
         <f t="shared" ref="K5" si="12">K4-(K1/$AZ$1)*$AZ$4</f>
-        <v>0.7896568898582712</v>
+        <v>0.85495145855120647</v>
       </c>
       <c r="L5">
         <f t="shared" ref="L5" si="13">L4-(L1/$AZ$1)*$AZ$4</f>
-        <v>0.74595782630329577</v>
+        <v>0.82315872843738225</v>
       </c>
       <c r="M5">
         <f t="shared" ref="M5" si="14">M4-(M1/$AZ$1)*$AZ$4</f>
-        <v>0.70024559290603894</v>
+        <v>0.78919514579760264</v>
       </c>
       <c r="N5">
         <f t="shared" ref="N5" si="15">N4-(N1/$AZ$1)*$AZ$4</f>
-        <v>0.65318086706370559</v>
+        <v>0.75341121032991965</v>
       </c>
       <c r="O5">
         <f t="shared" ref="O5" si="16">O4-(O1/$AZ$1)*$AZ$4</f>
-        <v>0.60541228559032623</v>
+        <v>0.71616885247691531</v>
       </c>
       <c r="P5">
         <f t="shared" ref="P5" si="17">P4-(P1/$AZ$1)*$AZ$4</f>
-        <v>0.55756090541472048</v>
+        <v>0.67783463691464085</v>
       </c>
       <c r="Q5">
         <f t="shared" ref="Q5" si="18">Q4-(Q1/$AZ$1)*$AZ$4</f>
-        <v>0.51020655045680308</v>
+        <v>0.63877318933354366</v>
       </c>
       <c r="R5">
         <f t="shared" ref="R5" si="19">R4-(R1/$AZ$1)*$AZ$4</f>
-        <v>0.46387640977843403</v>
+        <v>0.59934098860138396</v>
       </c>
       <c r="S5">
         <f t="shared" ref="S5" si="20">S4-(S1/$AZ$1)*$AZ$4</f>
-        <v>0.41903613712911153</v>
+        <v>0.55988065530948361</v>
       </c>
       <c r="T5">
         <f t="shared" ref="T5" si="21">T4-(T1/$AZ$1)*$AZ$4</f>
-        <v>0.37608357997374359</v>
+        <v>0.52071585050298785</v>
       </c>
       <c r="U5">
         <f t="shared" ref="U5" si="22">U4-(U1/$AZ$1)*$AZ$4</f>
-        <v>0.33534514534346171</v>
+        <v>0.48214687685948071</v>
       </c>
       <c r="V5">
         <f t="shared" ref="V5" si="23">V4-(V1/$AZ$1)*$AZ$4</f>
-        <v>0.29707469759139959</v>
+        <v>0.44444705022232817</v>
       </c>
       <c r="W5">
         <f t="shared" ref="W5" si="24">W4-(W1/$AZ$1)*$AZ$4</f>
-        <v>0.26145478522685495</v>
+        <v>0.40785988357918684</v>
       </c>
       <c r="X5">
         <f t="shared" ref="X5" si="25">X4-(X1/$AZ$1)*$AZ$4</f>
-        <v>0.22859991478661795</v>
+        <v>0.37259709954565506</v>
       </c>
       <c r="Y5">
         <f t="shared" ref="Y5" si="26">Y4-(Y1/$AZ$1)*$AZ$4</f>
-        <v>0.19856153190022169</v>
+        <v>0.33883746228643769</v>
       </c>
       <c r="Z5">
         <f t="shared" ref="Z5" si="27">Z4-(Z1/$AZ$1)*$AZ$4</f>
-        <v>0.17133433441001086</v>
+        <v>0.30672639655315731</v>
       </c>
       <c r="AA5">
         <f t="shared" ref="AA5" si="28">AA4-(AA1/$AZ$1)*$AZ$4</f>
-        <v>0.14686352919211709</v>
+        <v>0.27637634094295721</v>
       </c>
       <c r="AB5">
         <f t="shared" ref="AB5" si="29">AB4-(AB1/$AZ$1)*$AZ$4</f>
-        <v>0.12505265144658254</v>
+        <v>0.24786776520364279</v>
       </c>
       <c r="AC5">
         <f t="shared" ref="AC5" si="30">AC4-(AC1/$AZ$1)*$AZ$4</f>
-        <v>0.10577158989206685</v>
+        <v>0.22125076785169923</v>
       </c>
       <c r="AD5">
         <f t="shared" ref="AD5" si="31">AD4-(AD1/$AZ$1)*$AZ$4</f>
-        <v>8.8864499987292248E-2</v>
+        <v>0.19654716075401762</v>
       </c>
       <c r="AE5">
         <f t="shared" ref="AE5" si="32">AE4-(AE1/$AZ$1)*$AZ$4</f>
-        <v>7.4157336077313535E-2</v>
+        <v>0.17375294168734828</v>
       </c>
       <c r="AF5">
         <f t="shared" ref="AF5" si="33">AF4-(AF1/$AZ$1)*$AZ$4</f>
-        <v>6.1464788208541732E-2</v>
+        <v>0.15284105409201892</v>
       </c>
       <c r="AG5">
         <f t="shared" ref="AG5:AY5" si="34">AG4-(AG1/$AZ$1)*$AZ$4</f>
-        <v>5.059646644403528E-2</v>
+        <v>0.13376433498753743</v>
       </c>
       <c r="AH5">
         <f t="shared" si="34"/>
-        <v>4.1362231430190508E-2</v>
+        <v>0.11645855690355962</v>
       </c>
       <c r="AI5">
         <f t="shared" si="34"/>
-        <v>3.3576621890530858E-2</v>
+        <v>0.10084547719503707</v>
       </c>
       <c r="AJ5">
         <f t="shared" si="34"/>
-        <v>2.7062375504946036E-2</v>
+        <v>8.6835817691422193E-2</v>
       </c>
       <c r="AK5">
         <f t="shared" si="34"/>
-        <v>2.1653077840251611E-2</v>
+        <v>7.4332108686899406E-2</v>
       </c>
       <c r="AL5">
         <f t="shared" si="34"/>
-        <v>1.71950038876151E-2</v>
+        <v>6.3231343226248543E-2</v>
       </c>
       <c r="AM5">
         <f t="shared" si="34"/>
-        <v>1.3548238213365971E-2</v>
+        <v>5.3427399924593527E-2</v>
       </c>
       <c r="AN5">
         <f t="shared" si="34"/>
-        <v>1.0587173141721484E-2</v>
+        <v>4.4813204677238122E-2</v>
       </c>
       <c r="AO5">
         <f t="shared" si="34"/>
-        <v>8.2004905611868569E-3</v>
+        <v>3.7282613135834669E-2</v>
       </c>
       <c r="AP5">
         <f t="shared" si="34"/>
-        <v>6.2907329547424728E-3</v>
+        <v>3.0732006397685231E-2</v>
       </c>
       <c r="AQ5">
         <f t="shared" si="34"/>
-        <v>4.7735643231080708E-3</v>
+        <v>2.506160171065961E-2</v>
       </c>
       <c r="AR5">
         <f t="shared" si="34"/>
-        <v>3.5768130687120923E-3</v>
+        <v>2.0176487958429617E-2</v>
       </c>
       <c r="AS5">
         <f t="shared" si="34"/>
-        <v>2.6393778563279071E-3</v>
+        <v>1.5987402163804773E-2</v>
       </c>
       <c r="AT5">
         <f t="shared" si="34"/>
-        <v>1.9100650694817479E-3</v>
+        <v>1.241126821170134E-2</v>
       </c>
       <c r="AU5">
         <f t="shared" si="34"/>
-        <v>1.3464136827143758E-3</v>
+        <v>9.3715224928235703E-3</v>
       </c>
       <c r="AV5">
         <f t="shared" si="34"/>
-        <v>9.1355092504765692E-4</v>
+        <v>6.7982533030589345E-3</v>
       </c>
       <c r="AW5">
         <f t="shared" si="34"/>
-        <v>5.8311058327258363E-4</v>
+        <v>4.6281817411675192E-3</v>
       </c>
       <c r="AX5">
         <f t="shared" si="34"/>
-        <v>3.3223556439938574E-4</v>
+        <v>2.8045116958390582E-3</v>
       </c>
       <c r="AY5">
         <f t="shared" si="34"/>
-        <v>1.4267761930706339E-4</v>
+        <v>1.2766754856562406E-3</v>
       </c>
       <c r="AZ5">
         <v>0</v>
@@ -8324,207 +8332,207 @@
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B6">
         <f>B5/SUM($B$5:$AZ$5)</f>
-        <v>6.0192694283551618E-2</v>
+        <v>4.9941081907415655E-2</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:AZ6" si="35">C5/SUM($B$5:$AZ$5)</f>
-        <v>6.0035289835080566E-2</v>
+        <v>4.9852160520590598E-2</v>
       </c>
       <c r="D6">
         <f t="shared" si="35"/>
-        <v>5.9544449970861169E-2</v>
+        <v>4.9581767885936025E-2</v>
       </c>
       <c r="E6">
         <f t="shared" si="35"/>
-        <v>5.8715306239949035E-2</v>
+        <v>4.9124221909465797E-2</v>
       </c>
       <c r="F6">
         <f t="shared" si="35"/>
-        <v>5.755505173321445E-2</v>
+        <v>4.8479967596651581E-2</v>
       </c>
       <c r="G6">
         <f t="shared" si="35"/>
-        <v>5.6078928671239994E-2</v>
+        <v>4.7653108874577611E-2</v>
       </c>
       <c r="H6">
         <f t="shared" si="35"/>
-        <v>5.4308830141498857E-2</v>
+        <v>4.6650707228810789E-2</v>
       </c>
       <c r="I6">
         <f t="shared" si="35"/>
-        <v>5.2272253912054589E-2</v>
+        <v>4.5482377562410338E-2</v>
       </c>
       <c r="J6">
         <f t="shared" si="35"/>
-        <v>5.0001290290909842E-2</v>
+        <v>4.415995931128211E-2</v>
       </c>
       <c r="K6">
         <f t="shared" si="35"/>
-        <v>4.7531575760139111E-2</v>
+        <v>4.2697200818370286E-2</v>
       </c>
       <c r="L6">
         <f t="shared" si="35"/>
-        <v>4.4901211387096983E-2</v>
+        <v>4.1109437479695428E-2</v>
       </c>
       <c r="M6">
         <f t="shared" si="35"/>
-        <v>4.2149668897197547E-2</v>
+        <v>3.9413259417212916E-2</v>
       </c>
       <c r="N6">
         <f t="shared" si="35"/>
-        <v>3.9316716243030805E-2</v>
+        <v>3.7626170965051685E-2</v>
       </c>
       <c r="O6">
         <f t="shared" si="35"/>
-        <v>3.644139662204475E-2</v>
+        <v>3.576624732108951E-2</v>
       </c>
       <c r="P6">
         <f t="shared" si="35"/>
-        <v>3.356109312408851E-2</v>
+        <v>3.3851795121837433E-2</v>
       </c>
       <c r="Q6">
         <f t="shared" si="35"/>
-        <v>3.0710706913111802E-2</v>
+        <v>3.1901024168767632E-2</v>
       </c>
       <c r="R6">
         <f t="shared" si="35"/>
-        <v>2.7921970919144796E-2</v>
+        <v>2.993173740221319E-2</v>
       </c>
       <c r="S6">
         <f t="shared" si="35"/>
-        <v>2.5222914095973024E-2</v>
+        <v>2.7961045665188474E-2</v>
       </c>
       <c r="T6">
         <f t="shared" si="35"/>
-        <v>2.2637483954423183E-2</v>
+        <v>2.6005112940459322E-2</v>
       </c>
       <c r="U6">
         <f t="shared" si="35"/>
-        <v>2.0185327813132176E-2</v>
+        <v>2.4078936668643976E-2</v>
       </c>
       <c r="V6">
         <f t="shared" si="35"/>
-        <v>1.7881726451497666E-2</v>
+        <v>2.2196166538662569E-2</v>
       </c>
       <c r="W6">
         <f t="shared" si="35"/>
-        <v>1.573766795613173E-2</v>
+        <v>2.0368963852577183E-2</v>
       </c>
       <c r="X6">
         <f t="shared" si="35"/>
-        <v>1.3760044783996846E-2</v>
+        <v>1.8607902266875063E-2</v>
       </c>
       <c r="Y6">
         <f t="shared" si="35"/>
-        <v>1.1951953586143727E-2</v>
+        <v>1.6921909457347849E-2</v>
       </c>
       <c r="Z6">
         <f t="shared" si="35"/>
-        <v>1.0313075211417583E-2</v>
+        <v>1.5318248093427685E-2</v>
       </c>
       <c r="AA6">
         <f t="shared" si="35"/>
-        <v>8.8401115140645629E-3</v>
+        <v>1.3802533480304061E-2</v>
       </c>
       <c r="AB6">
         <f t="shared" si="35"/>
-        <v>7.527256017871682E-3</v>
+        <v>1.2378784364243197E-2</v>
       </c>
       <c r="AC6">
         <f t="shared" si="35"/>
-        <v>6.3666769742583788E-3</v>
+        <v>1.1049502719360317E-2</v>
       </c>
       <c r="AD6">
         <f t="shared" si="35"/>
-        <v>5.3489936803957595E-3</v>
+        <v>9.8157778538863864E-3</v>
       </c>
       <c r="AE6">
         <f t="shared" si="35"/>
-        <v>4.4637298593843263E-3</v>
+        <v>8.6774098924622765E-3</v>
       </c>
       <c r="AF6">
         <f t="shared" si="35"/>
-        <v>3.6997312058400008E-3</v>
+        <v>7.6330476012252636E-3</v>
       </c>
       <c r="AG6">
         <f t="shared" si="35"/>
-        <v>3.0455376364937939E-3</v>
+        <v>6.680335609903592E-3</v>
       </c>
       <c r="AH6">
         <f t="shared" si="35"/>
-        <v>2.4897041513629674E-3</v>
+        <v>5.8160663291400979E-3</v>
       </c>
       <c r="AI6">
         <f t="shared" si="35"/>
-        <v>2.0210673365311312E-3</v>
+        <v>5.0363322365897644E-3</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="35"/>
-        <v>1.6289572953558926E-3</v>
+        <v>4.336674683824729E-3</v>
       </c>
       <c r="AK6">
         <f t="shared" si="35"/>
-        <v>1.3033570947362115E-3</v>
+        <v>3.712225928283366E-3</v>
       </c>
       <c r="AL6">
         <f t="shared" si="35"/>
-        <v>1.0350136122116973E-3</v>
+        <v>3.1578416911779905E-3</v>
       </c>
       <c r="AM6">
         <f t="shared" si="35"/>
-        <v>8.155049608578695E-4</v>
+        <v>2.6682221557343786E-3</v>
       </c>
       <c r="AN6">
         <f t="shared" si="35"/>
-        <v>6.3727047624667003E-4</v>
+        <v>2.2380199253197314E-3</v>
       </c>
       <c r="AO6">
         <f t="shared" si="35"/>
-        <v>4.9360962132467118E-4</v>
+        <v>1.8619340363392101E-3</v>
       </c>
       <c r="AP6">
         <f t="shared" si="35"/>
-        <v>3.7865616556427702E-4</v>
+        <v>1.53478964868602E-3</v>
       </c>
       <c r="AQ6">
         <f t="shared" si="35"/>
-        <v>2.8733369794371315E-4</v>
+        <v>1.2516035037630799E-3</v>
       </c>
       <c r="AR6">
         <f t="shared" si="35"/>
-        <v>2.1529801555439907E-4</v>
+        <v>1.0076356377359192E-3</v>
       </c>
       <c r="AS6">
         <f t="shared" si="35"/>
-        <v>1.5887126440472155E-4</v>
+        <v>7.9842816094936842E-4</v>
       </c>
       <c r="AT6">
         <f t="shared" si="35"/>
-        <v>1.1497196278900563E-4</v>
+        <v>6.1983216233548084E-4</v>
       </c>
       <c r="AU6">
         <f t="shared" si="35"/>
-        <v>8.1044267182817299E-5</v>
+        <v>4.6802397241129008E-4</v>
       </c>
       <c r="AV6">
         <f t="shared" si="35"/>
-        <v>5.4989091543849397E-5</v>
+        <v>3.395121250354253E-4</v>
       </c>
       <c r="AW6">
         <f t="shared" si="35"/>
-        <v>3.5098997072430095E-5</v>
+        <v>2.3113640341805268E-4</v>
       </c>
       <c r="AX6">
         <f t="shared" si="35"/>
-        <v>1.9998153758015452E-5</v>
+        <v>1.4006034831220358E-4</v>
       </c>
       <c r="AY6">
         <f t="shared" si="35"/>
-        <v>8.5881503200550279E-6</v>
+        <v>6.3758554998347974E-5</v>
       </c>
       <c r="AZ6">
         <f t="shared" si="35"/>
@@ -8533,206 +8541,206 @@
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
         <f>(B5-C5)/B5</f>
-        <v>2.6150091858251345E-3</v>
+        <v>1.7805258402272539E-3</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:AZ7" si="36">(C5-D5)/C5</f>
-        <v>8.1758556603583749E-3</v>
+        <v>5.4238899945548685E-3</v>
       </c>
       <c r="E7">
         <f t="shared" si="36"/>
-        <v>1.3924786127303026E-2</v>
+        <v>9.2281093631599309E-3</v>
       </c>
       <c r="F7">
         <f t="shared" si="36"/>
-        <v>1.9760682197466944E-2</v>
+        <v>1.3114799334665243E-2</v>
       </c>
       <c r="G7">
         <f t="shared" si="36"/>
-        <v>2.5647150293891575E-2</v>
+        <v>1.7055678109221407E-2</v>
       </c>
       <c r="H7">
         <f t="shared" si="36"/>
-        <v>3.1564414151316167E-2</v>
+        <v>2.1035388234692781E-2</v>
       </c>
       <c r="I7">
         <f t="shared" si="36"/>
-        <v>3.7499909759390417E-2</v>
+        <v>2.5044200523478943E-2</v>
       </c>
       <c r="J7">
         <f t="shared" si="36"/>
-        <v>4.3444914867561142E-2</v>
+        <v>2.9075398473037677E-2</v>
       </c>
       <c r="K7">
         <f t="shared" si="36"/>
-        <v>4.939301598822373E-2</v>
+        <v>3.3124090595303565E-2</v>
       </c>
       <c r="L7">
         <f t="shared" si="36"/>
-        <v>5.533930510353504E-2</v>
+        <v>3.7186590882832007E-2</v>
       </c>
       <c r="M7">
         <f t="shared" si="36"/>
-        <v>6.1279916619134567E-2</v>
+        <v>4.1260064998950227E-2</v>
       </c>
       <c r="N7">
         <f t="shared" si="36"/>
-        <v>6.7211741593422109E-2</v>
+        <v>4.5342315722834106E-2</v>
       </c>
       <c r="O7">
         <f t="shared" si="36"/>
-        <v>7.3132242357491523E-2</v>
+        <v>4.943164813899685E-2</v>
       </c>
       <c r="P7">
         <f t="shared" si="36"/>
-        <v>7.9039327933272382E-2</v>
+        <v>5.3526784123175901E-2</v>
       </c>
       <c r="Q7">
         <f t="shared" si="36"/>
-        <v>8.4931268491098139E-2</v>
+        <v>5.7626809628520313E-2</v>
       </c>
       <c r="R7">
         <f t="shared" si="36"/>
-        <v>9.0806636325794512E-2</v>
+        <v>6.1731145562481743E-2</v>
       </c>
       <c r="S7">
         <f t="shared" si="36"/>
-        <v>9.6664265964160612E-2</v>
+        <v>6.5839537162283163E-2</v>
       </c>
       <c r="T7">
         <f t="shared" si="36"/>
-        <v>0.10250322907623978</v>
+        <v>6.9952059309580428E-2</v>
       </c>
       <c r="U7">
         <f t="shared" si="36"/>
-        <v>0.10832282183956567</v>
+        <v>7.4069136951086217E-2</v>
       </c>
       <c r="V7">
         <f t="shared" si="36"/>
-        <v>0.11412256382261145</v>
+        <v>7.8191581127134355E-2</v>
       </c>
       <c r="W7">
         <f t="shared" si="36"/>
-        <v>0.11990220861399896</v>
+        <v>8.2320642301122543E-2</v>
       </c>
       <c r="X7">
         <f t="shared" si="36"/>
-        <v>0.12566176752791119</v>
+        <v>8.6458083899014881E-2</v>
       </c>
       <c r="Y7">
         <f t="shared" si="36"/>
-        <v>0.13140154892198885</v>
+        <v>9.0606280350501611E-2</v>
       </c>
       <c r="Z7">
         <f t="shared" si="36"/>
-        <v>0.13712221712659151</v>
+        <v>9.4768345615028685E-2</v>
       </c>
       <c r="AA7">
         <f t="shared" si="36"/>
-        <v>0.14282487688272696</v>
+        <v>9.8948300346039089E-2</v>
       </c>
       <c r="AB7">
         <f t="shared" si="36"/>
-        <v>0.14851119175410132</v>
+        <v>0.10315128871757681</v>
       </c>
       <c r="AC7">
         <f t="shared" si="36"/>
-        <v>0.15418354854116612</v>
+        <v>0.10738385981765565</v>
       </c>
       <c r="AD7">
         <f t="shared" si="36"/>
-        <v>0.1598452847501603</v>
+        <v>0.11165433384728421</v>
       </c>
       <c r="AE7">
         <f t="shared" si="36"/>
-        <v>0.1655010033487147</v>
+        <v>0.11597328081068911</v>
       </c>
       <c r="AF7">
         <f t="shared" si="36"/>
-        <v>0.17115700940954851</v>
+        <v>0.12035414993409603</v>
       </c>
       <c r="AG7">
         <f t="shared" si="36"/>
-        <v>0.17682191839060279</v>
+        <v>0.1248141032382323</v>
       </c>
       <c r="AH7">
         <f t="shared" si="36"/>
-        <v>0.18250750818851658</v>
+        <v>0.12937512892050151</v>
       </c>
       <c r="AI7">
         <f t="shared" si="36"/>
-        <v>0.18822992064148872</v>
+        <v>0.13406554334562018</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="36"/>
-        <v>0.19401136918487752</v>
+        <v>0.13892204086178234</v>
       </c>
       <c r="AK7">
         <f t="shared" si="36"/>
-        <v>0.1998825884189582</v>
+        <v>0.14399252908466512</v>
       </c>
       <c r="AL7">
         <f t="shared" si="36"/>
-        <v>0.2058863864770879</v>
+        <v>0.14934011232493538</v>
       </c>
       <c r="AM7">
         <f t="shared" si="36"/>
-        <v>0.2120828641903218</v>
+        <v>0.15504879070140029</v>
       </c>
       <c r="AN7">
         <f t="shared" si="36"/>
-        <v>0.21855720463515754</v>
+        <v>0.16123178854882186</v>
       </c>
       <c r="AO7">
         <f t="shared" si="36"/>
-        <v>0.22543152441035361</v>
+        <v>0.16804403067447776</v>
       </c>
       <c r="AP7">
         <f t="shared" si="36"/>
-        <v>0.23288333694124572</v>
+        <v>0.17570138429629648</v>
       </c>
       <c r="AQ7">
         <f t="shared" si="36"/>
-        <v>0.24117517665260854</v>
+        <v>0.184511372724845</v>
       </c>
       <c r="AR7">
         <f t="shared" si="36"/>
-        <v>0.25070391292366057</v>
+        <v>0.19492424341546283</v>
       </c>
       <c r="AS7">
         <f t="shared" si="36"/>
-        <v>0.26208672199962879</v>
+        <v>0.20762214926878136</v>
       </c>
       <c r="AT7">
         <f t="shared" si="36"/>
-        <v>0.27631996119753455</v>
+        <v>0.22368449329433546</v>
       </c>
       <c r="AU7">
         <f t="shared" si="36"/>
-        <v>0.29509538485005954</v>
+        <v>0.244918220042324</v>
       </c>
       <c r="AV7">
         <f t="shared" si="36"/>
-        <v>0.32149313633984</v>
+        <v>0.27458389943951667</v>
       </c>
       <c r="AW7">
         <f t="shared" si="36"/>
-        <v>0.36170982122078776</v>
+        <v>0.31921016548691594</v>
       </c>
       <c r="AX7">
         <f t="shared" si="36"/>
-        <v>0.43023574956437149</v>
+        <v>0.39403596213756642</v>
       </c>
       <c r="AY7">
         <f t="shared" si="36"/>
-        <v>0.57055284082847824</v>
+        <v>0.54477797773124181</v>
       </c>
       <c r="AZ7">
         <f t="shared" si="36"/>
@@ -8750,15 +8758,22 @@
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B10" s="16">
-        <v>2.0499999999999998</v>
-      </c>
+        <v>2.06</v>
+      </c>
+      <c r="AS10" s="21"/>
+      <c r="AT10" s="21"/>
+      <c r="AU10" s="21"/>
+      <c r="AV10" s="21"/>
+      <c r="AW10" s="21"/>
+      <c r="AX10" s="21"/>
+      <c r="AY10" s="21"/>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>13</v>
@@ -8766,10 +8781,10 @@
     </row>
     <row r="12" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B12" s="19">
-        <v>18.2</v>
+        <v>22.2</v>
       </c>
     </row>
   </sheetData>
@@ -8782,7 +8797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165B24ED-3B36-4DB8-86F8-D9B901C367F8}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -8796,13 +8811,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -9373,642 +9388,642 @@
   <sheetData>
     <row r="1" spans="1:211" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AH1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AI1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AK1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AL1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AM1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AN1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AO1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AP1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AR1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AQ1" s="8" t="s">
+      <c r="AS1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AT1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="AS1" s="8" t="s">
+      <c r="AU1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AV1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="AU1" s="8" t="s">
+      <c r="AW1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="AV1" s="8" t="s">
+      <c r="AX1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AW1" s="8" t="s">
+      <c r="AY1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="AX1" s="8" t="s">
+      <c r="AZ1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="AY1" s="8" t="s">
+      <c r="BA1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="AZ1" s="8" t="s">
+      <c r="BB1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="BA1" s="8" t="s">
+      <c r="BC1" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="BB1" s="8" t="s">
+      <c r="BD1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="BC1" s="8" t="s">
+      <c r="BE1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="BD1" s="8" t="s">
+      <c r="BF1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="BE1" s="8" t="s">
+      <c r="BG1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="BF1" s="8" t="s">
+      <c r="BH1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="BG1" s="8" t="s">
+      <c r="BI1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="BH1" s="8" t="s">
+      <c r="BJ1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="BI1" s="8" t="s">
+      <c r="BK1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="BJ1" s="8" t="s">
+      <c r="BL1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="BK1" s="8" t="s">
+      <c r="BM1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="BL1" s="8" t="s">
+      <c r="BN1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="BM1" s="8" t="s">
+      <c r="BO1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="BN1" s="8" t="s">
+      <c r="BP1" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="BO1" s="8" t="s">
+      <c r="BQ1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="BP1" s="8" t="s">
+      <c r="BR1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="BQ1" s="8" t="s">
+      <c r="BS1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="BR1" s="8" t="s">
+      <c r="BT1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="BS1" s="8" t="s">
+      <c r="BU1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="BT1" s="8" t="s">
+      <c r="BV1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="BU1" s="8" t="s">
+      <c r="BW1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="BV1" s="8" t="s">
+      <c r="BX1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="BW1" s="8" t="s">
+      <c r="BY1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="BX1" s="8" t="s">
+      <c r="BZ1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="BY1" s="8" t="s">
+      <c r="CA1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="BZ1" s="8" t="s">
+      <c r="CB1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="CA1" s="8" t="s">
+      <c r="CC1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="CB1" s="8" t="s">
+      <c r="CD1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="CC1" s="8" t="s">
+      <c r="CE1" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="CD1" s="8" t="s">
+      <c r="CF1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="CE1" s="8" t="s">
+      <c r="CG1" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="CF1" s="8" t="s">
+      <c r="CH1" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="CG1" s="8" t="s">
+      <c r="CI1" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="CH1" s="8" t="s">
+      <c r="CJ1" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="CI1" s="8" t="s">
+      <c r="CK1" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="CJ1" s="8" t="s">
+      <c r="CL1" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="CK1" s="8" t="s">
+      <c r="CM1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="CL1" s="8" t="s">
+      <c r="CN1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="CM1" s="8" t="s">
+      <c r="CO1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="CN1" s="8" t="s">
+      <c r="CP1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="CO1" s="8" t="s">
+      <c r="CQ1" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="CP1" s="8" t="s">
+      <c r="CR1" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="CQ1" s="8" t="s">
+      <c r="CS1" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="CR1" s="8" t="s">
+      <c r="CT1" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="CS1" s="8" t="s">
+      <c r="CU1" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="CV1" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="CW1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CX1" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="CW1" s="8" t="s">
+      <c r="CY1" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="CX1" s="8" t="s">
+      <c r="CZ1" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="CY1" s="8" t="s">
+      <c r="DA1" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="CZ1" s="8" t="s">
+      <c r="DB1" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="DA1" s="8" t="s">
+      <c r="DC1" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="DB1" s="8" t="s">
+      <c r="DD1" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="DC1" s="8" t="s">
+      <c r="DE1" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="DD1" s="8" t="s">
+      <c r="DF1" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="DE1" s="8" t="s">
+      <c r="DG1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="DF1" s="8" t="s">
+      <c r="DH1" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="DG1" s="8" t="s">
+      <c r="DI1" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="DH1" s="8" t="s">
+      <c r="DJ1" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="DI1" s="8" t="s">
+      <c r="DK1" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="DJ1" s="8" t="s">
+      <c r="DL1" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="DK1" s="8" t="s">
+      <c r="DM1" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="DL1" s="8" t="s">
+      <c r="DN1" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="DM1" s="8" t="s">
+      <c r="DO1" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="DN1" s="8" t="s">
+      <c r="DP1" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="DO1" s="8" t="s">
+      <c r="DQ1" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="DP1" s="8" t="s">
+      <c r="DR1" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="DQ1" s="8" t="s">
+      <c r="DS1" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="DR1" s="8" t="s">
+      <c r="DT1" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="DS1" s="8" t="s">
+      <c r="DU1" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="DT1" s="8" t="s">
+      <c r="DV1" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="DU1" s="8" t="s">
+      <c r="DW1" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="DV1" s="8" t="s">
+      <c r="DX1" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="DW1" s="8" t="s">
+      <c r="DY1" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="DX1" s="8" t="s">
+      <c r="DZ1" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="DY1" s="8" t="s">
+      <c r="EA1" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="DZ1" s="8" t="s">
+      <c r="EB1" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="EA1" s="8" t="s">
+      <c r="EC1" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="EB1" s="8" t="s">
+      <c r="ED1" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="EC1" s="8" t="s">
+      <c r="EE1" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="ED1" s="8" t="s">
+      <c r="EF1" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="EE1" s="8" t="s">
+      <c r="EG1" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="EF1" s="8" t="s">
+      <c r="EH1" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="EG1" s="8" t="s">
+      <c r="EI1" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="EH1" s="8" t="s">
+      <c r="EJ1" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="EI1" s="8" t="s">
+      <c r="EK1" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="EJ1" s="8" t="s">
+      <c r="EL1" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="EK1" s="8" t="s">
+      <c r="EM1" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="EL1" s="8" t="s">
+      <c r="EN1" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="EM1" s="8" t="s">
+      <c r="EO1" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="EN1" s="8" t="s">
+      <c r="EP1" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="EO1" s="8" t="s">
+      <c r="EQ1" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="EP1" s="8" t="s">
+      <c r="ER1" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="EQ1" s="8" t="s">
+      <c r="ES1" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="ER1" s="8" t="s">
+      <c r="ET1" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="ES1" s="8" t="s">
+      <c r="EU1" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="ET1" s="8" t="s">
+      <c r="EV1" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="EU1" s="8" t="s">
+      <c r="EW1" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="EV1" s="8" t="s">
+      <c r="EX1" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="EW1" s="8" t="s">
+      <c r="EY1" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="EX1" s="8" t="s">
+      <c r="EZ1" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="EY1" s="8" t="s">
+      <c r="FA1" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="EZ1" s="8" t="s">
+      <c r="FB1" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="FA1" s="8" t="s">
+      <c r="FC1" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="FB1" s="8" t="s">
+      <c r="FD1" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="FC1" s="8" t="s">
+      <c r="FE1" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="FD1" s="8" t="s">
+      <c r="FF1" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="FE1" s="8" t="s">
+      <c r="FG1" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="FF1" s="8" t="s">
+      <c r="FH1" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="FG1" s="8" t="s">
+      <c r="FI1" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="FH1" s="8" t="s">
+      <c r="FJ1" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="FI1" s="8" t="s">
+      <c r="FK1" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="FJ1" s="8" t="s">
+      <c r="FL1" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="FK1" s="8" t="s">
+      <c r="FM1" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="FL1" s="8" t="s">
+      <c r="FN1" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="FM1" s="8" t="s">
+      <c r="FO1" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="FN1" s="8" t="s">
+      <c r="FP1" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="FO1" s="8" t="s">
+      <c r="FQ1" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="FP1" s="8" t="s">
+      <c r="FR1" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="FQ1" s="8" t="s">
+      <c r="FS1" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="FR1" s="8" t="s">
+      <c r="FT1" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="FS1" s="8" t="s">
+      <c r="FU1" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="FT1" s="8" t="s">
+      <c r="FV1" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="FU1" s="8" t="s">
+      <c r="FW1" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="FV1" s="8" t="s">
+      <c r="FX1" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="FW1" s="8" t="s">
+      <c r="FY1" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="FX1" s="8" t="s">
+      <c r="FZ1" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="FY1" s="8" t="s">
+      <c r="GA1" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="FZ1" s="8" t="s">
+      <c r="GB1" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="GA1" s="8" t="s">
+      <c r="GC1" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="GB1" s="8" t="s">
+      <c r="GD1" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="GC1" s="8" t="s">
+      <c r="GE1" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="GD1" s="8" t="s">
+      <c r="GF1" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="GE1" s="8" t="s">
+      <c r="GG1" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="GF1" s="8" t="s">
+      <c r="GH1" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="GG1" s="8" t="s">
+      <c r="GI1" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="GH1" s="8" t="s">
+      <c r="GJ1" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="GI1" s="8" t="s">
+      <c r="GK1" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="GJ1" s="8" t="s">
+      <c r="GL1" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="GK1" s="8" t="s">
+      <c r="GM1" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="GL1" s="8" t="s">
+      <c r="GN1" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="GM1" s="8" t="s">
+      <c r="GO1" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="GN1" s="8" t="s">
+      <c r="GP1" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="GO1" s="8" t="s">
+      <c r="GQ1" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="GP1" s="8" t="s">
+      <c r="GR1" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="GQ1" s="8" t="s">
+      <c r="GS1" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="GR1" s="8" t="s">
+      <c r="GT1" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="GS1" s="8" t="s">
+      <c r="GU1" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="GT1" s="8" t="s">
+      <c r="GV1" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="GU1" s="8" t="s">
+      <c r="GW1" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="GV1" s="8" t="s">
+      <c r="GX1" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="GW1" s="8" t="s">
+      <c r="GY1" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="GX1" s="8" t="s">
+      <c r="GZ1" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="GY1" s="8" t="s">
+      <c r="HA1" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="GZ1" s="8" t="s">
+      <c r="HB1" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="HA1" s="8" t="s">
+      <c r="HC1" s="8" t="s">
         <v>233</v>
-      </c>
-      <c r="HB1" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="HC1" s="8" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:211" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -10252,203 +10267,203 @@
       </c>
       <c r="CD2" cm="1">
         <f t="array" ref="CD2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CE2:$HC2,"&gt;0")+1)</f>
-        <v>8.5881503200550279E-6</v>
+        <v>6.3758554998347974E-5</v>
       </c>
       <c r="CE2" cm="1">
         <f t="array" ref="CE2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CF2:$HC2,"&gt;0")+1)</f>
-        <v>1.9998153758015452E-5</v>
+        <v>1.4006034831220358E-4</v>
       </c>
       <c r="CF2" cm="1">
         <f t="array" ref="CF2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CG2:$HC2,"&gt;0")+1)</f>
-        <v>3.5098997072430095E-5</v>
+        <v>2.3113640341805268E-4</v>
       </c>
       <c r="CG2" cm="1">
         <f t="array" ref="CG2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CH2:$HC2,"&gt;0")+1)</f>
-        <v>5.4989091543849397E-5</v>
+        <v>3.395121250354253E-4</v>
       </c>
       <c r="CH2" cm="1">
         <f t="array" ref="CH2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CI2:$HC2,"&gt;0")+1)</f>
-        <v>8.1044267182817299E-5</v>
+        <v>4.6802397241129008E-4</v>
       </c>
       <c r="CI2" cm="1">
         <f t="array" ref="CI2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CJ2:$HC2,"&gt;0")+1)</f>
-        <v>1.1497196278900563E-4</v>
+        <v>6.1983216233548084E-4</v>
       </c>
       <c r="CJ2" cm="1">
         <f t="array" ref="CJ2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CK2:$HC2,"&gt;0")+1)</f>
-        <v>1.5887126440472155E-4</v>
+        <v>7.9842816094936842E-4</v>
       </c>
       <c r="CK2" cm="1">
         <f t="array" ref="CK2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CL2:$HC2,"&gt;0")+1)</f>
-        <v>2.1529801555439907E-4</v>
+        <v>1.0076356377359192E-3</v>
       </c>
       <c r="CL2" cm="1">
         <f t="array" ref="CL2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CM2:$HC2,"&gt;0")+1)</f>
-        <v>2.8733369794371315E-4</v>
+        <v>1.2516035037630799E-3</v>
       </c>
       <c r="CM2" cm="1">
         <f t="array" ref="CM2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CN2:$HC2,"&gt;0")+1)</f>
-        <v>3.7865616556427702E-4</v>
+        <v>1.53478964868602E-3</v>
       </c>
       <c r="CN2" cm="1">
         <f t="array" ref="CN2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CO2:$HC2,"&gt;0")+1)</f>
-        <v>4.9360962132467118E-4</v>
+        <v>1.8619340363392101E-3</v>
       </c>
       <c r="CO2" cm="1">
         <f t="array" ref="CO2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CP2:$HC2,"&gt;0")+1)</f>
-        <v>6.3727047624667003E-4</v>
+        <v>2.2380199253197314E-3</v>
       </c>
       <c r="CP2" cm="1">
         <f t="array" ref="CP2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CQ2:$HC2,"&gt;0")+1)</f>
-        <v>8.155049608578695E-4</v>
+        <v>2.6682221557343786E-3</v>
       </c>
       <c r="CQ2" cm="1">
         <f t="array" ref="CQ2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CR2:$HC2,"&gt;0")+1)</f>
-        <v>1.0350136122116973E-3</v>
+        <v>3.1578416911779905E-3</v>
       </c>
       <c r="CR2" cm="1">
         <f t="array" ref="CR2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CS2:$HC2,"&gt;0")+1)</f>
-        <v>1.3033570947362115E-3</v>
+        <v>3.712225928283366E-3</v>
       </c>
       <c r="CS2" cm="1">
         <f t="array" ref="CS2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CT2:$HC2,"&gt;0")+1)</f>
-        <v>1.6289572953558926E-3</v>
+        <v>4.336674683824729E-3</v>
       </c>
       <c r="CT2" cm="1">
         <f t="array" ref="CT2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CU2:$HC2,"&gt;0")+1)</f>
-        <v>2.0210673365311312E-3</v>
+        <v>5.0363322365897644E-3</v>
       </c>
       <c r="CU2" cm="1">
         <f t="array" ref="CU2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CV2:$HC2,"&gt;0")+1)</f>
-        <v>2.4897041513629674E-3</v>
+        <v>5.8160663291400979E-3</v>
       </c>
       <c r="CV2" cm="1">
         <f t="array" ref="CV2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CW2:$HC2,"&gt;0")+1)</f>
-        <v>3.0455376364937939E-3</v>
+        <v>6.680335609903592E-3</v>
       </c>
       <c r="CW2" cm="1">
         <f t="array" ref="CW2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CX2:$HC2,"&gt;0")+1)</f>
-        <v>3.6997312058400008E-3</v>
+        <v>7.6330476012252636E-3</v>
       </c>
       <c r="CX2" cm="1">
         <f t="array" ref="CX2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CY2:$HC2,"&gt;0")+1)</f>
-        <v>4.4637298593843263E-3</v>
+        <v>8.6774098924622765E-3</v>
       </c>
       <c r="CY2" cm="1">
         <f t="array" ref="CY2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(CZ2:$HC2,"&gt;0")+1)</f>
-        <v>5.3489936803957595E-3</v>
+        <v>9.8157778538863864E-3</v>
       </c>
       <c r="CZ2" cm="1">
         <f t="array" ref="CZ2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DA2:$HC2,"&gt;0")+1)</f>
-        <v>6.3666769742583788E-3</v>
+        <v>1.1049502719360317E-2</v>
       </c>
       <c r="DA2" cm="1">
         <f t="array" ref="DA2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DB2:$HC2,"&gt;0")+1)</f>
-        <v>7.527256017871682E-3</v>
+        <v>1.2378784364243197E-2</v>
       </c>
       <c r="DB2" cm="1">
         <f t="array" ref="DB2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DC2:$HC2,"&gt;0")+1)</f>
-        <v>8.8401115140645629E-3</v>
+        <v>1.3802533480304061E-2</v>
       </c>
       <c r="DC2" cm="1">
         <f t="array" ref="DC2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DD2:$HC2,"&gt;0")+1)</f>
-        <v>1.0313075211417583E-2</v>
+        <v>1.5318248093427685E-2</v>
       </c>
       <c r="DD2" cm="1">
         <f t="array" ref="DD2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DE2:$HC2,"&gt;0")+1)</f>
-        <v>1.1951953586143727E-2</v>
+        <v>1.6921909457347849E-2</v>
       </c>
       <c r="DE2" cm="1">
         <f t="array" ref="DE2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DF2:$HC2,"&gt;0")+1)</f>
-        <v>1.3760044783996846E-2</v>
+        <v>1.8607902266875063E-2</v>
       </c>
       <c r="DF2" cm="1">
         <f t="array" ref="DF2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DG2:$HC2,"&gt;0")+1)</f>
-        <v>1.573766795613173E-2</v>
+        <v>2.0368963852577183E-2</v>
       </c>
       <c r="DG2" cm="1">
         <f t="array" ref="DG2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DH2:$HC2,"&gt;0")+1)</f>
-        <v>1.7881726451497666E-2</v>
+        <v>2.2196166538662569E-2</v>
       </c>
       <c r="DH2" cm="1">
         <f t="array" ref="DH2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DI2:$HC2,"&gt;0")+1)</f>
-        <v>2.0185327813132176E-2</v>
+        <v>2.4078936668643976E-2</v>
       </c>
       <c r="DI2" cm="1">
         <f t="array" ref="DI2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DJ2:$HC2,"&gt;0")+1)</f>
-        <v>2.2637483954423183E-2</v>
+        <v>2.6005112940459322E-2</v>
       </c>
       <c r="DJ2" cm="1">
         <f t="array" ref="DJ2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DK2:$HC2,"&gt;0")+1)</f>
-        <v>2.5222914095973024E-2</v>
+        <v>2.7961045665188474E-2</v>
       </c>
       <c r="DK2" cm="1">
         <f t="array" ref="DK2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DL2:$HC2,"&gt;0")+1)</f>
-        <v>2.7921970919144796E-2</v>
+        <v>2.993173740221319E-2</v>
       </c>
       <c r="DL2" cm="1">
         <f t="array" ref="DL2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DM2:$HC2,"&gt;0")+1)</f>
-        <v>3.0710706913111802E-2</v>
+        <v>3.1901024168767632E-2</v>
       </c>
       <c r="DM2" cm="1">
         <f t="array" ref="DM2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DN2:$HC2,"&gt;0")+1)</f>
-        <v>3.356109312408851E-2</v>
+        <v>3.3851795121837433E-2</v>
       </c>
       <c r="DN2" cm="1">
         <f t="array" ref="DN2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DO2:$HC2,"&gt;0")+1)</f>
-        <v>3.644139662204475E-2</v>
+        <v>3.576624732108951E-2</v>
       </c>
       <c r="DO2" cm="1">
         <f t="array" ref="DO2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DP2:$HC2,"&gt;0")+1)</f>
-        <v>3.9316716243030805E-2</v>
+        <v>3.7626170965051685E-2</v>
       </c>
       <c r="DP2" cm="1">
         <f t="array" ref="DP2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DQ2:$HC2,"&gt;0")+1)</f>
-        <v>4.2149668897197547E-2</v>
+        <v>3.9413259417212916E-2</v>
       </c>
       <c r="DQ2" cm="1">
         <f t="array" ref="DQ2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DR2:$HC2,"&gt;0")+1)</f>
-        <v>4.4901211387096983E-2</v>
+        <v>4.1109437479695428E-2</v>
       </c>
       <c r="DR2" cm="1">
         <f t="array" ref="DR2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DS2:$HC2,"&gt;0")+1)</f>
-        <v>4.7531575760139111E-2</v>
+        <v>4.2697200818370286E-2</v>
       </c>
       <c r="DS2" cm="1">
         <f t="array" ref="DS2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DT2:$HC2,"&gt;0")+1)</f>
-        <v>5.0001290290909842E-2</v>
+        <v>4.415995931128211E-2</v>
       </c>
       <c r="DT2" cm="1">
         <f t="array" ref="DT2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DU2:$HC2,"&gt;0")+1)</f>
-        <v>5.2272253912054589E-2</v>
+        <v>4.5482377562410338E-2</v>
       </c>
       <c r="DU2" cm="1">
         <f t="array" ref="DU2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DV2:$HC2,"&gt;0")+1)</f>
-        <v>5.4308830141498857E-2</v>
+        <v>4.6650707228810789E-2</v>
       </c>
       <c r="DV2" cm="1">
         <f t="array" ref="DV2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DW2:$HC2,"&gt;0")+1)</f>
-        <v>5.6078928671239994E-2</v>
+        <v>4.7653108874577611E-2</v>
       </c>
       <c r="DW2" cm="1">
         <f t="array" ref="DW2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DX2:$HC2,"&gt;0")+1)</f>
-        <v>5.755505173321445E-2</v>
+        <v>4.8479967596651581E-2</v>
       </c>
       <c r="DX2" cm="1">
         <f t="array" ref="DX2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DY2:$HC2,"&gt;0")+1)</f>
-        <v>5.8715306239949035E-2</v>
+        <v>4.9124221909465797E-2</v>
       </c>
       <c r="DY2" cm="1">
         <f t="array" ref="DY2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(DZ2:$HC2,"&gt;0")+1)</f>
-        <v>5.9544449970861169E-2</v>
+        <v>4.9581767885936025E-2</v>
       </c>
       <c r="DZ2" cm="1">
         <f t="array" ref="DZ2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(EA2:$HC2,"&gt;0")+1)</f>
-        <v>6.0035289835080566E-2</v>
+        <v>4.9852160520590598E-2</v>
       </c>
       <c r="EA2" cm="1">
         <f t="array" ref="EA2">INDEX(Calculations!$B$6:$AZ$6,COUNTIF(EB2:$HC2,"&gt;0")+1)</f>
-        <v>6.0192694283551618E-2</v>
+        <v>4.9941081907415655E-2</v>
       </c>
       <c r="EB2">
         <v>0</v>
@@ -10704,7 +10719,9 @@
   </sheetPr>
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -10713,7 +10730,7 @@
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -10871,7 +10888,7 @@
     </row>
     <row r="2" spans="1:52" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B2">
         <f>Calculations!B7</f>
@@ -10879,199 +10896,199 @@
       </c>
       <c r="C2">
         <f>Calculations!C7</f>
-        <v>2.6150091858251345E-3</v>
+        <v>1.7805258402272539E-3</v>
       </c>
       <c r="D2">
         <f>Calculations!D7</f>
-        <v>8.1758556603583749E-3</v>
+        <v>5.4238899945548685E-3</v>
       </c>
       <c r="E2">
         <f>Calculations!E7</f>
-        <v>1.3924786127303026E-2</v>
+        <v>9.2281093631599309E-3</v>
       </c>
       <c r="F2">
         <f>Calculations!F7</f>
-        <v>1.9760682197466944E-2</v>
+        <v>1.3114799334665243E-2</v>
       </c>
       <c r="G2">
         <f>Calculations!G7</f>
-        <v>2.5647150293891575E-2</v>
+        <v>1.7055678109221407E-2</v>
       </c>
       <c r="H2">
         <f>Calculations!H7</f>
-        <v>3.1564414151316167E-2</v>
+        <v>2.1035388234692781E-2</v>
       </c>
       <c r="I2">
         <f>Calculations!I7</f>
-        <v>3.7499909759390417E-2</v>
+        <v>2.5044200523478943E-2</v>
       </c>
       <c r="J2">
         <f>Calculations!J7</f>
-        <v>4.3444914867561142E-2</v>
+        <v>2.9075398473037677E-2</v>
       </c>
       <c r="K2">
         <f>Calculations!K7</f>
-        <v>4.939301598822373E-2</v>
+        <v>3.3124090595303565E-2</v>
       </c>
       <c r="L2">
         <f>Calculations!L7</f>
-        <v>5.533930510353504E-2</v>
+        <v>3.7186590882832007E-2</v>
       </c>
       <c r="M2">
         <f>Calculations!M7</f>
-        <v>6.1279916619134567E-2</v>
+        <v>4.1260064998950227E-2</v>
       </c>
       <c r="N2">
         <f>Calculations!N7</f>
-        <v>6.7211741593422109E-2</v>
+        <v>4.5342315722834106E-2</v>
       </c>
       <c r="O2">
         <f>Calculations!O7</f>
-        <v>7.3132242357491523E-2</v>
+        <v>4.943164813899685E-2</v>
       </c>
       <c r="P2">
         <f>Calculations!P7</f>
-        <v>7.9039327933272382E-2</v>
+        <v>5.3526784123175901E-2</v>
       </c>
       <c r="Q2">
         <f>Calculations!Q7</f>
-        <v>8.4931268491098139E-2</v>
+        <v>5.7626809628520313E-2</v>
       </c>
       <c r="R2">
         <f>Calculations!R7</f>
-        <v>9.0806636325794512E-2</v>
+        <v>6.1731145562481743E-2</v>
       </c>
       <c r="S2">
         <f>Calculations!S7</f>
-        <v>9.6664265964160612E-2</v>
+        <v>6.5839537162283163E-2</v>
       </c>
       <c r="T2">
         <f>Calculations!T7</f>
-        <v>0.10250322907623978</v>
+        <v>6.9952059309580428E-2</v>
       </c>
       <c r="U2">
         <f>Calculations!U7</f>
-        <v>0.10832282183956567</v>
+        <v>7.4069136951086217E-2</v>
       </c>
       <c r="V2">
         <f>Calculations!V7</f>
-        <v>0.11412256382261145</v>
+        <v>7.8191581127134355E-2</v>
       </c>
       <c r="W2">
         <f>Calculations!W7</f>
-        <v>0.11990220861399896</v>
+        <v>8.2320642301122543E-2</v>
       </c>
       <c r="X2">
         <f>Calculations!X7</f>
-        <v>0.12566176752791119</v>
+        <v>8.6458083899014881E-2</v>
       </c>
       <c r="Y2">
         <f>Calculations!Y7</f>
-        <v>0.13140154892198885</v>
+        <v>9.0606280350501611E-2</v>
       </c>
       <c r="Z2">
         <f>Calculations!Z7</f>
-        <v>0.13712221712659151</v>
+        <v>9.4768345615028685E-2</v>
       </c>
       <c r="AA2">
         <f>Calculations!AA7</f>
-        <v>0.14282487688272696</v>
+        <v>9.8948300346039089E-2</v>
       </c>
       <c r="AB2">
         <f>Calculations!AB7</f>
-        <v>0.14851119175410132</v>
+        <v>0.10315128871757681</v>
       </c>
       <c r="AC2">
         <f>Calculations!AC7</f>
-        <v>0.15418354854116612</v>
+        <v>0.10738385981765565</v>
       </c>
       <c r="AD2">
         <f>Calculations!AD7</f>
-        <v>0.1598452847501603</v>
+        <v>0.11165433384728421</v>
       </c>
       <c r="AE2">
         <f>Calculations!AE7</f>
-        <v>0.1655010033487147</v>
+        <v>0.11597328081068911</v>
       </c>
       <c r="AF2">
         <f>Calculations!AF7</f>
-        <v>0.17115700940954851</v>
+        <v>0.12035414993409603</v>
       </c>
       <c r="AG2">
         <f>Calculations!AG7</f>
-        <v>0.17682191839060279</v>
+        <v>0.1248141032382323</v>
       </c>
       <c r="AH2">
         <f>Calculations!AH7</f>
-        <v>0.18250750818851658</v>
+        <v>0.12937512892050151</v>
       </c>
       <c r="AI2">
         <f>Calculations!AI7</f>
-        <v>0.18822992064148872</v>
+        <v>0.13406554334562018</v>
       </c>
       <c r="AJ2">
         <f>Calculations!AJ7</f>
-        <v>0.19401136918487752</v>
+        <v>0.13892204086178234</v>
       </c>
       <c r="AK2">
         <f>Calculations!AK7</f>
-        <v>0.1998825884189582</v>
+        <v>0.14399252908466512</v>
       </c>
       <c r="AL2">
         <f>Calculations!AL7</f>
-        <v>0.2058863864770879</v>
+        <v>0.14934011232493538</v>
       </c>
       <c r="AM2">
         <f>Calculations!AM7</f>
-        <v>0.2120828641903218</v>
+        <v>0.15504879070140029</v>
       </c>
       <c r="AN2">
         <f>Calculations!AN7</f>
-        <v>0.21855720463515754</v>
+        <v>0.16123178854882186</v>
       </c>
       <c r="AO2">
         <f>Calculations!AO7</f>
-        <v>0.22543152441035361</v>
+        <v>0.16804403067447776</v>
       </c>
       <c r="AP2">
         <f>Calculations!AP7</f>
-        <v>0.23288333694124572</v>
+        <v>0.17570138429629648</v>
       </c>
       <c r="AQ2">
         <f>Calculations!AQ7</f>
-        <v>0.24117517665260854</v>
+        <v>0.184511372724845</v>
       </c>
       <c r="AR2">
         <f>Calculations!AR7</f>
-        <v>0.25070391292366057</v>
+        <v>0.19492424341546283</v>
       </c>
       <c r="AS2">
         <f>Calculations!AS7</f>
-        <v>0.26208672199962879</v>
+        <v>0.20762214926878136</v>
       </c>
       <c r="AT2">
         <f>Calculations!AT7</f>
-        <v>0.27631996119753455</v>
+        <v>0.22368449329433546</v>
       </c>
       <c r="AU2">
         <f>Calculations!AU7</f>
-        <v>0.29509538485005954</v>
+        <v>0.244918220042324</v>
       </c>
       <c r="AV2">
         <f>Calculations!AV7</f>
-        <v>0.32149313633984</v>
+        <v>0.27458389943951667</v>
       </c>
       <c r="AW2">
         <f>Calculations!AW7</f>
-        <v>0.36170982122078776</v>
+        <v>0.31921016548691594</v>
       </c>
       <c r="AX2">
         <f>Calculations!AX7</f>
-        <v>0.43023574956437149</v>
+        <v>0.39403596213756642</v>
       </c>
       <c r="AY2">
         <f>Calculations!AY7</f>
-        <v>0.57055284082847824</v>
+        <v>0.54477797773124181</v>
       </c>
       <c r="AZ2">
         <f>Calculations!AZ7</f>

</xml_diff>